<commit_message>
Added some crossed values
</commit_message>
<xml_diff>
--- a/usa.xlsx
+++ b/usa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="398">
   <si>
     <t>date</t>
   </si>
@@ -1202,6 +1202,9 @@
   </si>
   <si>
     <t>2021-02-16</t>
+  </si>
+  <si>
+    <t>2021-02-17</t>
   </si>
   <si>
     <t>united states of america</t>
@@ -1562,7 +1565,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E393"/>
+  <dimension ref="A1:E394"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1590,7 +1593,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1607,7 +1610,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1624,7 +1627,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1641,7 +1644,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1658,7 +1661,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1675,7 +1678,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1692,7 +1695,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1709,7 +1712,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -1726,7 +1729,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -1743,7 +1746,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D11">
         <v>8</v>
@@ -1760,7 +1763,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D12">
         <v>8</v>
@@ -1777,7 +1780,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -1794,7 +1797,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D14">
         <v>11</v>
@@ -1811,7 +1814,7 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -1828,7 +1831,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D16">
         <v>11</v>
@@ -1845,7 +1848,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D17">
         <v>12</v>
@@ -1862,7 +1865,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D18">
         <v>12</v>
@@ -1879,7 +1882,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D19">
         <v>12</v>
@@ -1896,7 +1899,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D20">
         <v>12</v>
@@ -1913,7 +1916,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D21">
         <v>12</v>
@@ -1930,7 +1933,7 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D22">
         <v>13</v>
@@ -1947,7 +1950,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D23">
         <v>13</v>
@@ -1964,7 +1967,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D24">
         <v>14</v>
@@ -1981,7 +1984,7 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D25">
         <v>14</v>
@@ -1998,7 +2001,7 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D26">
         <v>14</v>
@@ -2015,7 +2018,7 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D27">
         <v>14</v>
@@ -2032,7 +2035,7 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D28">
         <v>14</v>
@@ -2049,7 +2052,7 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D29">
         <v>14</v>
@@ -2066,7 +2069,7 @@
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D30">
         <v>14</v>
@@ -2083,7 +2086,7 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D31">
         <v>14</v>
@@ -2100,7 +2103,7 @@
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D32">
         <v>16</v>
@@ -2117,7 +2120,7 @@
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D33">
         <v>16</v>
@@ -2134,7 +2137,7 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D34">
         <v>16</v>
@@ -2151,7 +2154,7 @@
         <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D35">
         <v>16</v>
@@ -2168,7 +2171,7 @@
         <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D36">
         <v>16</v>
@@ -2185,7 +2188,7 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D37">
         <v>16</v>
@@ -2202,7 +2205,7 @@
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D38">
         <v>17</v>
@@ -2219,7 +2222,7 @@
         <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D39">
         <v>17</v>
@@ -2236,7 +2239,7 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D40">
         <v>25</v>
@@ -2253,7 +2256,7 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D41">
         <v>32</v>
@@ -2270,7 +2273,7 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D42">
         <v>55</v>
@@ -2287,7 +2290,7 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D43">
         <v>74</v>
@@ -2304,7 +2307,7 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D44">
         <v>107</v>
@@ -2321,7 +2324,7 @@
         <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D45">
         <v>184</v>
@@ -2338,7 +2341,7 @@
         <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D46">
         <v>237</v>
@@ -2355,7 +2358,7 @@
         <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D47">
         <v>403</v>
@@ -2372,7 +2375,7 @@
         <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D48">
         <v>519</v>
@@ -2389,7 +2392,7 @@
         <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D49">
         <v>594</v>
@@ -2406,7 +2409,7 @@
         <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D50">
         <v>782</v>
@@ -2423,7 +2426,7 @@
         <v>53</v>
       </c>
       <c r="C51" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D51">
         <v>1147</v>
@@ -2440,7 +2443,7 @@
         <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D52">
         <v>1586</v>
@@ -2457,7 +2460,7 @@
         <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D53">
         <v>2219</v>
@@ -2474,7 +2477,7 @@
         <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D54">
         <v>2978</v>
@@ -2491,7 +2494,7 @@
         <v>57</v>
       </c>
       <c r="C55" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D55">
         <v>3212</v>
@@ -2508,7 +2511,7 @@
         <v>58</v>
       </c>
       <c r="C56" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D56">
         <v>4679</v>
@@ -2525,7 +2528,7 @@
         <v>59</v>
       </c>
       <c r="C57" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D57">
         <v>6512</v>
@@ -2542,7 +2545,7 @@
         <v>60</v>
       </c>
       <c r="C58" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D58">
         <v>9169</v>
@@ -2559,7 +2562,7 @@
         <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D59">
         <v>13663</v>
@@ -2576,7 +2579,7 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D60">
         <v>20030</v>
@@ -2593,7 +2596,7 @@
         <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D61">
         <v>26025</v>
@@ -2610,7 +2613,7 @@
         <v>64</v>
       </c>
       <c r="C62" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D62">
         <v>34898</v>
@@ -2627,7 +2630,7 @@
         <v>65</v>
       </c>
       <c r="C63" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D63">
         <v>46136</v>
@@ -2644,7 +2647,7 @@
         <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D64">
         <v>56755</v>
@@ -2661,7 +2664,7 @@
         <v>67</v>
       </c>
       <c r="C65" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D65">
         <v>68837</v>
@@ -2678,7 +2681,7 @@
         <v>68</v>
       </c>
       <c r="C66" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D66">
         <v>86693</v>
@@ -2695,7 +2698,7 @@
         <v>69</v>
       </c>
       <c r="C67" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D67">
         <v>105383</v>
@@ -2712,7 +2715,7 @@
         <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D68">
         <v>125013</v>
@@ -2729,7 +2732,7 @@
         <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D69">
         <v>143912</v>
@@ -2746,7 +2749,7 @@
         <v>72</v>
       </c>
       <c r="C70" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D70">
         <v>165987</v>
@@ -2763,7 +2766,7 @@
         <v>73</v>
       </c>
       <c r="C71" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D71">
         <v>192301</v>
@@ -2780,7 +2783,7 @@
         <v>74</v>
       </c>
       <c r="C72" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D72">
         <v>224544</v>
@@ -2797,7 +2800,7 @@
         <v>75</v>
       </c>
       <c r="C73" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D73">
         <v>256779</v>
@@ -2814,7 +2817,7 @@
         <v>76</v>
       </c>
       <c r="C74" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D74">
         <v>289066</v>
@@ -2831,7 +2834,7 @@
         <v>77</v>
       </c>
       <c r="C75" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D75">
         <v>321482</v>
@@ -2848,7 +2851,7 @@
         <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D76">
         <v>351359</v>
@@ -2865,7 +2868,7 @@
         <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D77">
         <v>382740</v>
@@ -2882,7 +2885,7 @@
         <v>80</v>
       </c>
       <c r="C78" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D78">
         <v>413507</v>
@@ -2899,7 +2902,7 @@
         <v>81</v>
       </c>
       <c r="C79" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D79">
         <v>444699</v>
@@ -2916,7 +2919,7 @@
         <v>82</v>
       </c>
       <c r="C80" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D80">
         <v>480640</v>
@@ -2933,7 +2936,7 @@
         <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D81">
         <v>515055</v>
@@ -2950,7 +2953,7 @@
         <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D82">
         <v>544185</v>
@@ -2967,7 +2970,7 @@
         <v>85</v>
       </c>
       <c r="C83" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D83">
         <v>571440</v>
@@ -2984,7 +2987,7 @@
         <v>86</v>
       </c>
       <c r="C84" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D84">
         <v>598370</v>
@@ -3001,7 +3004,7 @@
         <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D85">
         <v>627151</v>
@@ -3018,7 +3021,7 @@
         <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D86">
         <v>652591</v>
@@ -3035,7 +3038,7 @@
         <v>89</v>
       </c>
       <c r="C87" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D87">
         <v>682626</v>
@@ -3052,7 +3055,7 @@
         <v>90</v>
       </c>
       <c r="C88" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D88">
         <v>715656</v>
@@ -3069,7 +3072,7 @@
         <v>91</v>
       </c>
       <c r="C89" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D89">
         <v>743588</v>
@@ -3086,7 +3089,7 @@
         <v>92</v>
       </c>
       <c r="C90" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D90">
         <v>769684</v>
@@ -3103,7 +3106,7 @@
         <v>93</v>
       </c>
       <c r="C91" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D91">
         <v>799512</v>
@@ -3120,7 +3123,7 @@
         <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D92">
         <v>825429</v>
@@ -3137,7 +3140,7 @@
         <v>95</v>
       </c>
       <c r="C93" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D93">
         <v>854288</v>
@@ -3154,7 +3157,7 @@
         <v>96</v>
       </c>
       <c r="C94" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D94">
         <v>887858</v>
@@ -3171,7 +3174,7 @@
         <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D95">
         <v>920185</v>
@@ -3188,7 +3191,7 @@
         <v>98</v>
       </c>
       <c r="C96" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D96">
         <v>950580</v>
@@ -3205,7 +3208,7 @@
         <v>99</v>
       </c>
       <c r="C97" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D97">
         <v>977081</v>
@@ -3222,7 +3225,7 @@
         <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D98">
         <v>1000784</v>
@@ -3239,7 +3242,7 @@
         <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D99">
         <v>1025361</v>
@@ -3256,7 +3259,7 @@
         <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D100">
         <v>1051799</v>
@@ -3273,7 +3276,7 @@
         <v>103</v>
       </c>
       <c r="C101" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D101">
         <v>1081019</v>
@@ -3290,7 +3293,7 @@
         <v>104</v>
       </c>
       <c r="C102" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D102">
         <v>1115945</v>
@@ -3307,7 +3310,7 @@
         <v>105</v>
       </c>
       <c r="C103" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D103">
         <v>1143295</v>
@@ -3324,7 +3327,7 @@
         <v>106</v>
       </c>
       <c r="C104" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D104">
         <v>1167592</v>
@@ -3341,7 +3344,7 @@
         <v>107</v>
       </c>
       <c r="C105" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D105">
         <v>1191677</v>
@@ -3358,7 +3361,7 @@
         <v>108</v>
       </c>
       <c r="C106" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D106">
         <v>1216208</v>
@@ -3375,7 +3378,7 @@
         <v>109</v>
       </c>
       <c r="C107" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D107">
         <v>1240767</v>
@@ -3392,7 +3395,7 @@
         <v>110</v>
       </c>
       <c r="C108" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D108">
         <v>1268179</v>
@@ -3409,7 +3412,7 @@
         <v>111</v>
       </c>
       <c r="C109" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D109">
         <v>1295017</v>
@@ -3426,7 +3429,7 @@
         <v>112</v>
       </c>
       <c r="C110" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D110">
         <v>1320153</v>
@@ -3443,7 +3446,7 @@
         <v>113</v>
       </c>
       <c r="C111" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D111">
         <v>1339020</v>
@@ -3460,7 +3463,7 @@
         <v>114</v>
       </c>
       <c r="C112" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D112">
         <v>1358291</v>
@@ -3477,7 +3480,7 @@
         <v>115</v>
       </c>
       <c r="C113" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D113">
         <v>1381238</v>
@@ -3494,7 +3497,7 @@
         <v>116</v>
       </c>
       <c r="C114" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D114">
         <v>1401646</v>
@@ -3511,7 +3514,7 @@
         <v>117</v>
       </c>
       <c r="C115" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D115">
         <v>1428464</v>
@@ -3528,7 +3531,7 @@
         <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D116">
         <v>1453211</v>
@@ -3545,7 +3548,7 @@
         <v>119</v>
       </c>
       <c r="C117" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D117">
         <v>1477370</v>
@@ -3562,7 +3565,7 @@
         <v>120</v>
       </c>
       <c r="C118" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D118">
         <v>1495733</v>
@@ -3579,7 +3582,7 @@
         <v>121</v>
       </c>
       <c r="C119" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D119">
         <v>1518123</v>
@@ -3596,7 +3599,7 @@
         <v>122</v>
       </c>
       <c r="C120" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D120">
         <v>1539130</v>
@@ -3613,7 +3616,7 @@
         <v>123</v>
       </c>
       <c r="C121" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D121">
         <v>1561827</v>
@@ -3630,7 +3633,7 @@
         <v>124</v>
       </c>
       <c r="C122" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D122">
         <v>1587593</v>
@@ -3647,7 +3650,7 @@
         <v>125</v>
       </c>
       <c r="C123" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D123">
         <v>1611249</v>
@@ -3664,7 +3667,7 @@
         <v>126</v>
       </c>
       <c r="C124" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D124">
         <v>1632361</v>
@@ -3681,7 +3684,7 @@
         <v>127</v>
       </c>
       <c r="C125" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D125">
         <v>1652428</v>
@@ -3698,7 +3701,7 @@
         <v>128</v>
       </c>
       <c r="C126" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D126">
         <v>1671100</v>
@@ -3715,7 +3718,7 @@
         <v>129</v>
       </c>
       <c r="C127" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D127">
         <v>1690750</v>
@@ -3732,7 +3735,7 @@
         <v>130</v>
       </c>
       <c r="C128" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D128">
         <v>1709299</v>
@@ -3749,7 +3752,7 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D129">
         <v>1731621</v>
@@ -3766,7 +3769,7 @@
         <v>132</v>
       </c>
       <c r="C130" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D130">
         <v>1756093</v>
@@ -3783,7 +3786,7 @@
         <v>133</v>
       </c>
       <c r="C131" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D131">
         <v>1779726</v>
@@ -3800,7 +3803,7 @@
         <v>134</v>
       </c>
       <c r="C132" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D132">
         <v>1798713</v>
@@ -3817,7 +3820,7 @@
         <v>135</v>
       </c>
       <c r="C133" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D133">
         <v>1816148</v>
@@ -3834,7 +3837,7 @@
         <v>136</v>
       </c>
       <c r="C134" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D134">
         <v>1837651</v>
@@ -3851,7 +3854,7 @@
         <v>137</v>
       </c>
       <c r="C135" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D135">
         <v>1857495</v>
@@ -3868,7 +3871,7 @@
         <v>138</v>
       </c>
       <c r="C136" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D136">
         <v>1879144</v>
@@ -3885,7 +3888,7 @@
         <v>139</v>
       </c>
       <c r="C137" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D137">
         <v>1904544</v>
@@ -3902,7 +3905,7 @@
         <v>140</v>
       </c>
       <c r="C138" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D138">
         <v>1925704</v>
@@ -3919,7 +3922,7 @@
         <v>141</v>
       </c>
       <c r="C139" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D139">
         <v>1943620</v>
@@ -3936,7 +3939,7 @@
         <v>142</v>
       </c>
       <c r="C140" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D140">
         <v>1961257</v>
@@ -3953,7 +3956,7 @@
         <v>143</v>
       </c>
       <c r="C141" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D141">
         <v>1979639</v>
@@ -3970,7 +3973,7 @@
         <v>144</v>
       </c>
       <c r="C142" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D142">
         <v>2000749</v>
@@ -3987,7 +3990,7 @@
         <v>145</v>
       </c>
       <c r="C143" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D143">
         <v>2023881</v>
@@ -4004,7 +4007,7 @@
         <v>146</v>
       </c>
       <c r="C144" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D144">
         <v>2048746</v>
@@ -4021,7 +4024,7 @@
         <v>147</v>
       </c>
       <c r="C145" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D145">
         <v>2073954</v>
@@ -4038,7 +4041,7 @@
         <v>148</v>
       </c>
       <c r="C146" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D146">
         <v>2092902</v>
@@ -4055,7 +4058,7 @@
         <v>149</v>
       </c>
       <c r="C147" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D147">
         <v>2112721</v>
@@ -4072,7 +4075,7 @@
         <v>150</v>
       </c>
       <c r="C148" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D148">
         <v>2136391</v>
@@ -4089,7 +4092,7 @@
         <v>151</v>
       </c>
       <c r="C149" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D149">
         <v>2163449</v>
@@ -4106,7 +4109,7 @@
         <v>152</v>
       </c>
       <c r="C150" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D150">
         <v>2191971</v>
@@ -4123,7 +4126,7 @@
         <v>153</v>
       </c>
       <c r="C151" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D151">
         <v>2223531</v>
@@ -4140,7 +4143,7 @@
         <v>154</v>
       </c>
       <c r="C152" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D152">
         <v>2255800</v>
@@ -4157,7 +4160,7 @@
         <v>155</v>
       </c>
       <c r="C153" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D153">
         <v>2280946</v>
@@ -4174,7 +4177,7 @@
         <v>156</v>
       </c>
       <c r="C154" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D154">
         <v>2313093</v>
@@ -4191,7 +4194,7 @@
         <v>157</v>
       </c>
       <c r="C155" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D155">
         <v>2350156</v>
@@ -4208,7 +4211,7 @@
         <v>158</v>
       </c>
       <c r="C156" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D156">
         <v>2386014</v>
@@ -4225,7 +4228,7 @@
         <v>159</v>
       </c>
       <c r="C157" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D157">
         <v>2426329</v>
@@ -4242,7 +4245,7 @@
         <v>160</v>
       </c>
       <c r="C158" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D158">
         <v>2472311</v>
@@ -4259,7 +4262,7 @@
         <v>161</v>
       </c>
       <c r="C159" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D159">
         <v>2513651</v>
@@ -4276,7 +4279,7 @@
         <v>162</v>
       </c>
       <c r="C160" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D160">
         <v>2554376</v>
@@ -4293,7 +4296,7 @@
         <v>163</v>
       </c>
       <c r="C161" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D161">
         <v>2595655</v>
@@ -4310,7 +4313,7 @@
         <v>164</v>
       </c>
       <c r="C162" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D162">
         <v>2642081</v>
@@ -4327,7 +4330,7 @@
         <v>165</v>
       </c>
       <c r="C163" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D163">
         <v>2693890</v>
@@ -4344,7 +4347,7 @@
         <v>166</v>
       </c>
       <c r="C164" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D164">
         <v>2750517</v>
@@ -4361,7 +4364,7 @@
         <v>167</v>
       </c>
       <c r="C165" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D165">
         <v>2801874</v>
@@ -4378,7 +4381,7 @@
         <v>168</v>
       </c>
       <c r="C166" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D166">
         <v>2847553</v>
@@ -4395,7 +4398,7 @@
         <v>169</v>
       </c>
       <c r="C167" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D167">
         <v>2898322</v>
@@ -4412,7 +4415,7 @@
         <v>170</v>
       </c>
       <c r="C168" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D168">
         <v>2941394</v>
@@ -4429,7 +4432,7 @@
         <v>171</v>
       </c>
       <c r="C169" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D169">
         <v>3002036</v>
@@ -4446,7 +4449,7 @@
         <v>172</v>
       </c>
       <c r="C170" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D170">
         <v>3062146</v>
@@ -4463,7 +4466,7 @@
         <v>173</v>
       </c>
       <c r="C171" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D171">
         <v>3124633</v>
@@ -4480,7 +4483,7 @@
         <v>174</v>
       </c>
       <c r="C172" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D172">
         <v>3192672</v>
@@ -4497,7 +4500,7 @@
         <v>175</v>
       </c>
       <c r="C173" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D173">
         <v>3252687</v>
@@ -4514,7 +4517,7 @@
         <v>176</v>
       </c>
       <c r="C174" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D174">
         <v>3311137</v>
@@ -4531,7 +4534,7 @@
         <v>177</v>
       </c>
       <c r="C175" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D175">
         <v>3370026</v>
@@ -4548,7 +4551,7 @@
         <v>178</v>
       </c>
       <c r="C176" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D176">
         <v>3438038</v>
@@ -4565,7 +4568,7 @@
         <v>179</v>
       </c>
       <c r="C177" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D177">
         <v>3506145</v>
@@ -4582,7 +4585,7 @@
         <v>180</v>
       </c>
       <c r="C178" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D178">
         <v>3581954</v>
@@ -4599,7 +4602,7 @@
         <v>181</v>
       </c>
       <c r="C179" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D179">
         <v>3654203</v>
@@ -4616,7 +4619,7 @@
         <v>182</v>
       </c>
       <c r="C180" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D180">
         <v>3716740</v>
@@ -4633,7 +4636,7 @@
         <v>183</v>
       </c>
       <c r="C181" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D181">
         <v>3777211</v>
@@ -4650,7 +4653,7 @@
         <v>184</v>
       </c>
       <c r="C182" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D182">
         <v>3839293</v>
@@ -4667,7 +4670,7 @@
         <v>185</v>
       </c>
       <c r="C183" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D183">
         <v>3903780</v>
@@ -4684,7 +4687,7 @@
         <v>186</v>
       </c>
       <c r="C184" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D184">
         <v>3974341</v>
@@ -4701,7 +4704,7 @@
         <v>187</v>
       </c>
       <c r="C185" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D185">
         <v>4042769</v>
@@ -4718,7 +4721,7 @@
         <v>188</v>
       </c>
       <c r="C186" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D186">
         <v>4116070</v>
@@ -4735,7 +4738,7 @@
         <v>189</v>
       </c>
       <c r="C187" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D187">
         <v>4180969</v>
@@ -4752,7 +4755,7 @@
         <v>190</v>
       </c>
       <c r="C188" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D188">
         <v>4235816</v>
@@ -4769,7 +4772,7 @@
         <v>191</v>
       </c>
       <c r="C189" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D189">
         <v>4292554</v>
@@ -4786,7 +4789,7 @@
         <v>192</v>
       </c>
       <c r="C190" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D190">
         <v>4359003</v>
@@ -4803,7 +4806,7 @@
         <v>193</v>
       </c>
       <c r="C191" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D191">
         <v>4430816</v>
@@ -4820,7 +4823,7 @@
         <v>194</v>
       </c>
       <c r="C192" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D192">
         <v>4498234</v>
@@ -4837,7 +4840,7 @@
         <v>195</v>
       </c>
       <c r="C193" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D193">
         <v>4566931</v>
@@ -4854,7 +4857,7 @@
         <v>196</v>
       </c>
       <c r="C194" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D194">
         <v>4623105</v>
@@ -4871,7 +4874,7 @@
         <v>197</v>
       </c>
       <c r="C195" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D195">
         <v>4668652</v>
@@ -4888,7 +4891,7 @@
         <v>198</v>
       </c>
       <c r="C196" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D196">
         <v>4714173</v>
@@ -4905,7 +4908,7 @@
         <v>199</v>
       </c>
       <c r="C197" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D197">
         <v>4772945</v>
@@ -4922,7 +4925,7 @@
         <v>200</v>
       </c>
       <c r="C198" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D198">
         <v>4827393</v>
@@ -4939,7 +4942,7 @@
         <v>201</v>
       </c>
       <c r="C199" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D199">
         <v>4886727</v>
@@ -4956,7 +4959,7 @@
         <v>202</v>
       </c>
       <c r="C200" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D200">
         <v>4945996</v>
@@ -4973,7 +4976,7 @@
         <v>203</v>
       </c>
       <c r="C201" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D201">
         <v>5000107</v>
@@ -4990,7 +4993,7 @@
         <v>204</v>
       </c>
       <c r="C202" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D202">
         <v>5045855</v>
@@ -5007,7 +5010,7 @@
         <v>205</v>
       </c>
       <c r="C203" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D203">
         <v>5093475</v>
@@ -5024,7 +5027,7 @@
         <v>206</v>
       </c>
       <c r="C204" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D204">
         <v>5141430</v>
@@ -5041,7 +5044,7 @@
         <v>207</v>
       </c>
       <c r="C205" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D205">
         <v>5197413</v>
@@ -5058,7 +5061,7 @@
         <v>208</v>
       </c>
       <c r="C206" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D206">
         <v>5248690</v>
@@ -5075,7 +5078,7 @@
         <v>209</v>
       </c>
       <c r="C207" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D207">
         <v>5314012</v>
@@ -5092,7 +5095,7 @@
         <v>210</v>
       </c>
       <c r="C208" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D208">
         <v>5360914</v>
@@ -5109,7 +5112,7 @@
         <v>211</v>
       </c>
       <c r="C209" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D209">
         <v>5400103</v>
@@ -5126,7 +5129,7 @@
         <v>212</v>
       </c>
       <c r="C210" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D210">
         <v>5436757</v>
@@ -5143,7 +5146,7 @@
         <v>213</v>
       </c>
       <c r="C211" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D211">
         <v>5481755</v>
@@ -5160,7 +5163,7 @@
         <v>214</v>
       </c>
       <c r="C212" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D212">
         <v>5529102</v>
@@ -5177,7 +5180,7 @@
         <v>215</v>
       </c>
       <c r="C213" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D213">
         <v>5572890</v>
@@ -5194,7 +5197,7 @@
         <v>216</v>
       </c>
       <c r="C214" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D214">
         <v>5621596</v>
@@ -5211,7 +5214,7 @@
         <v>217</v>
       </c>
       <c r="C215" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D215">
         <v>5664641</v>
@@ -5228,7 +5231,7 @@
         <v>218</v>
       </c>
       <c r="C216" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D216">
         <v>5698902</v>
@@ -5245,7 +5248,7 @@
         <v>219</v>
       </c>
       <c r="C217" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D217">
         <v>5735502</v>
@@ -5262,7 +5265,7 @@
         <v>220</v>
       </c>
       <c r="C218" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D218">
         <v>5775618</v>
@@ -5279,7 +5282,7 @@
         <v>221</v>
       </c>
       <c r="C219" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D219">
         <v>5820908</v>
@@ -5296,7 +5299,7 @@
         <v>222</v>
       </c>
       <c r="C220" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D220">
         <v>5866093</v>
@@ -5313,7 +5316,7 @@
         <v>223</v>
       </c>
       <c r="C221" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D221">
         <v>5913046</v>
@@ -5330,7 +5333,7 @@
         <v>224</v>
       </c>
       <c r="C222" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D222">
         <v>5955722</v>
@@ -5347,7 +5350,7 @@
         <v>225</v>
       </c>
       <c r="C223" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D223">
         <v>5990118</v>
@@ -5364,7 +5367,7 @@
         <v>226</v>
       </c>
       <c r="C224" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D224">
         <v>6025593</v>
@@ -5381,7 +5384,7 @@
         <v>227</v>
       </c>
       <c r="C225" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D225">
         <v>6067260</v>
@@ -5398,7 +5401,7 @@
         <v>228</v>
       </c>
       <c r="C226" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D226">
         <v>6108200</v>
@@ -5415,7 +5418,7 @@
         <v>229</v>
       </c>
       <c r="C227" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D227">
         <v>6152285</v>
@@ -5432,7 +5435,7 @@
         <v>230</v>
       </c>
       <c r="C228" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D228">
         <v>6202700</v>
@@ -5449,7 +5452,7 @@
         <v>231</v>
       </c>
       <c r="C229" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D229">
         <v>6245682</v>
@@ -5466,7 +5469,7 @@
         <v>232</v>
       </c>
       <c r="C230" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D230">
         <v>6276981</v>
@@ -5483,7 +5486,7 @@
         <v>233</v>
       </c>
       <c r="C231" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D231">
         <v>6300449</v>
@@ -5500,7 +5503,7 @@
         <v>234</v>
       </c>
       <c r="C232" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D232">
         <v>6327884</v>
@@ -5517,7 +5520,7 @@
         <v>235</v>
       </c>
       <c r="C233" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D233">
         <v>6361638</v>
@@ -5534,7 +5537,7 @@
         <v>236</v>
       </c>
       <c r="C234" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D234">
         <v>6397758</v>
@@ -5551,7 +5554,7 @@
         <v>237</v>
       </c>
       <c r="C235" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D235">
         <v>6445407</v>
@@ -5568,7 +5571,7 @@
         <v>238</v>
       </c>
       <c r="C236" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D236">
         <v>6486484</v>
@@ -5585,7 +5588,7 @@
         <v>239</v>
       </c>
       <c r="C237" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D237">
         <v>6520750</v>
@@ -5602,7 +5605,7 @@
         <v>240</v>
       </c>
       <c r="C238" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D238">
         <v>6555127</v>
@@ -5619,7 +5622,7 @@
         <v>241</v>
       </c>
       <c r="C239" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D239">
         <v>6594554</v>
@@ -5636,7 +5639,7 @@
         <v>242</v>
       </c>
       <c r="C240" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D240">
         <v>6633389</v>
@@ -5653,7 +5656,7 @@
         <v>243</v>
       </c>
       <c r="C241" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D241">
         <v>6678579</v>
@@ -5670,7 +5673,7 @@
         <v>244</v>
       </c>
       <c r="C242" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D242">
         <v>6727725</v>
@@ -5687,7 +5690,7 @@
         <v>245</v>
       </c>
       <c r="C243" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D243">
         <v>6769847</v>
@@ -5704,7 +5707,7 @@
         <v>246</v>
       </c>
       <c r="C244" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D244">
         <v>6808147</v>
@@ -5721,7 +5724,7 @@
         <v>247</v>
       </c>
       <c r="C245" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D245">
         <v>6860061</v>
@@ -5738,7 +5741,7 @@
         <v>248</v>
       </c>
       <c r="C246" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D246">
         <v>6899723</v>
@@ -5755,7 +5758,7 @@
         <v>249</v>
       </c>
       <c r="C247" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D247">
         <v>6938731</v>
@@ -5772,7 +5775,7 @@
         <v>250</v>
       </c>
       <c r="C248" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D248">
         <v>6985760</v>
@@ -5789,7 +5792,7 @@
         <v>251</v>
       </c>
       <c r="C249" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D249">
         <v>7033944</v>
@@ -5806,7 +5809,7 @@
         <v>252</v>
       </c>
       <c r="C250" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D250">
         <v>7078562</v>
@@ -5823,7 +5826,7 @@
         <v>253</v>
       </c>
       <c r="C251" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D251">
         <v>7116078</v>
@@ -5840,7 +5843,7 @@
         <v>254</v>
       </c>
       <c r="C252" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D252">
         <v>7149281</v>
@@ -5857,7 +5860,7 @@
         <v>255</v>
       </c>
       <c r="C253" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D253">
         <v>7192498</v>
@@ -5874,7 +5877,7 @@
         <v>256</v>
       </c>
       <c r="C254" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D254">
         <v>7231832</v>
@@ -5891,7 +5894,7 @@
         <v>257</v>
       </c>
       <c r="C255" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D255">
         <v>7277418</v>
@@ -5908,7 +5911,7 @@
         <v>258</v>
       </c>
       <c r="C256" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D256">
         <v>7332238</v>
@@ -5925,7 +5928,7 @@
         <v>259</v>
       </c>
       <c r="C257" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D257">
         <v>7380797</v>
@@ -5942,7 +5945,7 @@
         <v>260</v>
       </c>
       <c r="C258" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D258">
         <v>7416539</v>
@@ -5959,7 +5962,7 @@
         <v>261</v>
       </c>
       <c r="C259" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D259">
         <v>7455962</v>
@@ -5976,7 +5979,7 @@
         <v>262</v>
       </c>
       <c r="C260" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D260">
         <v>7501009</v>
@@ -5993,7 +5996,7 @@
         <v>263</v>
       </c>
       <c r="C261" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D261">
         <v>7551949</v>
@@ -6010,7 +6013,7 @@
         <v>264</v>
       </c>
       <c r="C262" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D262">
         <v>7610451</v>
@@ -6027,7 +6030,7 @@
         <v>265</v>
       </c>
       <c r="C263" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D263">
         <v>7666716</v>
@@ -6044,7 +6047,7 @@
         <v>266</v>
       </c>
       <c r="C264" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D264">
         <v>7721622</v>
@@ -6061,7 +6064,7 @@
         <v>267</v>
       </c>
       <c r="C265" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D265">
         <v>7767500</v>
@@ -6078,7 +6081,7 @@
         <v>268</v>
       </c>
       <c r="C266" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D266">
         <v>7809362</v>
@@ -6095,7 +6098,7 @@
         <v>269</v>
       </c>
       <c r="C267" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D267">
         <v>7861469</v>
@@ -6112,7 +6115,7 @@
         <v>270</v>
       </c>
       <c r="C268" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D268">
         <v>7921089</v>
@@ -6129,7 +6132,7 @@
         <v>271</v>
       </c>
       <c r="C269" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D269">
         <v>7985864</v>
@@ -6146,7 +6149,7 @@
         <v>272</v>
       </c>
       <c r="C270" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D270">
         <v>8054907</v>
@@ -6163,7 +6166,7 @@
         <v>273</v>
       </c>
       <c r="C271" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D271">
         <v>8111563</v>
@@ -6180,7 +6183,7 @@
         <v>274</v>
       </c>
       <c r="C272" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D272">
         <v>8160870</v>
@@ -6197,7 +6200,7 @@
         <v>275</v>
       </c>
       <c r="C273" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D273">
         <v>8228585</v>
@@ -6214,7 +6217,7 @@
         <v>276</v>
       </c>
       <c r="C274" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D274">
         <v>8290408</v>
@@ -6231,7 +6234,7 @@
         <v>277</v>
       </c>
       <c r="C275" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D275">
         <v>8353581</v>
@@ -6248,7 +6251,7 @@
         <v>278</v>
       </c>
       <c r="C276" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D276">
         <v>8429792</v>
@@ -6265,7 +6268,7 @@
         <v>279</v>
       </c>
       <c r="C277" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D277">
         <v>8511514</v>
@@ -6282,7 +6285,7 @@
         <v>280</v>
       </c>
       <c r="C278" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D278">
         <v>8594218</v>
@@ -6299,7 +6302,7 @@
         <v>281</v>
       </c>
       <c r="C279" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D279">
         <v>8656238</v>
@@ -6316,7 +6319,7 @@
         <v>282</v>
       </c>
       <c r="C280" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D280">
         <v>8723553</v>
@@ -6333,7 +6336,7 @@
         <v>283</v>
       </c>
       <c r="C281" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D281">
         <v>8800136</v>
@@ -6350,7 +6353,7 @@
         <v>284</v>
       </c>
       <c r="C282" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D282">
         <v>8879326</v>
@@ -6367,7 +6370,7 @@
         <v>285</v>
       </c>
       <c r="C283" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D283">
         <v>8970125</v>
@@ -6384,7 +6387,7 @@
         <v>286</v>
       </c>
       <c r="C284" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D284">
         <v>9069103</v>
@@ -6401,7 +6404,7 @@
         <v>287</v>
       </c>
       <c r="C285" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D285">
         <v>9158771</v>
@@ -6418,7 +6421,7 @@
         <v>288</v>
       </c>
       <c r="C286" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D286">
         <v>9263564</v>
@@ -6435,7 +6438,7 @@
         <v>289</v>
       </c>
       <c r="C287" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D287">
         <v>9348673</v>
@@ -6452,7 +6455,7 @@
         <v>290</v>
       </c>
       <c r="C288" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D288">
         <v>9475593</v>
@@ -6469,7 +6472,7 @@
         <v>291</v>
       </c>
       <c r="C289" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D289">
         <v>9579978</v>
@@ -6486,7 +6489,7 @@
         <v>292</v>
       </c>
       <c r="C290" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D290">
         <v>9709076</v>
@@ -6503,7 +6506,7 @@
         <v>293</v>
       </c>
       <c r="C291" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D291">
         <v>9836826</v>
@@ -6520,7 +6523,7 @@
         <v>294</v>
       </c>
       <c r="C292" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D292">
         <v>9964034</v>
@@ -6537,7 +6540,7 @@
         <v>295</v>
       </c>
       <c r="C293" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D293">
         <v>10079115</v>
@@ -6554,7 +6557,7 @@
         <v>296</v>
       </c>
       <c r="C294" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D294">
         <v>10199575</v>
@@ -6571,7 +6574,7 @@
         <v>297</v>
       </c>
       <c r="C295" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D295">
         <v>10339806</v>
@@ -6588,7 +6591,7 @@
         <v>298</v>
       </c>
       <c r="C296" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D296">
         <v>10486184</v>
@@ -6605,7 +6608,7 @@
         <v>299</v>
       </c>
       <c r="C297" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D297">
         <v>10650570</v>
@@ -6622,7 +6625,7 @@
         <v>300</v>
       </c>
       <c r="C298" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D298">
         <v>10830756</v>
@@ -6639,7 +6642,7 @@
         <v>301</v>
       </c>
       <c r="C299" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D299">
         <v>10998298</v>
@@ -6656,7 +6659,7 @@
         <v>302</v>
       </c>
       <c r="C300" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D300">
         <v>11134448</v>
@@ -6673,7 +6676,7 @@
         <v>303</v>
       </c>
       <c r="C301" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D301">
         <v>11296951</v>
@@ -6690,7 +6693,7 @@
         <v>304</v>
       </c>
       <c r="C302" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D302">
         <v>11460388</v>
@@ -6707,7 +6710,7 @@
         <v>305</v>
       </c>
       <c r="C303" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D303">
         <v>11633255</v>
@@ -6724,7 +6727,7 @@
         <v>306</v>
       </c>
       <c r="C304" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D304">
         <v>11824408</v>
@@ -6741,7 +6744,7 @@
         <v>307</v>
       </c>
       <c r="C305" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D305">
         <v>12022364</v>
@@ -6758,7 +6761,7 @@
         <v>308</v>
       </c>
       <c r="C306" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D306">
         <v>12201487</v>
@@ -6775,7 +6778,7 @@
         <v>309</v>
       </c>
       <c r="C307" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D307">
         <v>12348137</v>
@@ -6792,7 +6795,7 @@
         <v>310</v>
       </c>
       <c r="C308" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D308">
         <v>12522119</v>
@@ -6809,7 +6812,7 @@
         <v>311</v>
       </c>
       <c r="C309" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D309">
         <v>12697162</v>
@@ -6826,7 +6829,7 @@
         <v>312</v>
       </c>
       <c r="C310" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D310">
         <v>12879847</v>
@@ -6843,7 +6846,7 @@
         <v>313</v>
       </c>
       <c r="C311" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D311">
         <v>12991459</v>
@@ -6860,7 +6863,7 @@
         <v>314</v>
       </c>
       <c r="C312" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D312">
         <v>13199466</v>
@@ -6877,7 +6880,7 @@
         <v>315</v>
       </c>
       <c r="C313" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D313">
         <v>13354901</v>
@@ -6894,7 +6897,7 @@
         <v>316</v>
       </c>
       <c r="C314" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D314">
         <v>13494948</v>
@@ -6911,7 +6914,7 @@
         <v>317</v>
       </c>
       <c r="C315" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D315">
         <v>13655181</v>
@@ -6928,7 +6931,7 @@
         <v>318</v>
       </c>
       <c r="C316" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D316">
         <v>13842693</v>
@@ -6945,7 +6948,7 @@
         <v>319</v>
       </c>
       <c r="C317" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D317">
         <v>14044565</v>
@@ -6962,7 +6965,7 @@
         <v>320</v>
       </c>
       <c r="C318" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D318">
         <v>14266847</v>
@@ -6979,7 +6982,7 @@
         <v>321</v>
       </c>
       <c r="C319" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D319">
         <v>14498883</v>
@@ -6996,7 +6999,7 @@
         <v>322</v>
       </c>
       <c r="C320" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D320">
         <v>14713624</v>
@@ -7013,7 +7016,7 @@
         <v>323</v>
       </c>
       <c r="C321" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D321">
         <v>14894418</v>
@@ -7030,7 +7033,7 @@
         <v>324</v>
       </c>
       <c r="C322" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D322">
         <v>15089009</v>
@@ -7047,7 +7050,7 @@
         <v>325</v>
       </c>
       <c r="C323" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D323">
         <v>15312876</v>
@@ -7064,7 +7067,7 @@
         <v>326</v>
       </c>
       <c r="C324" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D324">
         <v>15534536</v>
@@ -7081,7 +7084,7 @@
         <v>327</v>
       </c>
       <c r="C325" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D325">
         <v>15765165</v>
@@ -7098,7 +7101,7 @@
         <v>328</v>
       </c>
       <c r="C326" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D326">
         <v>16003837</v>
@@ -7115,7 +7118,7 @@
         <v>329</v>
       </c>
       <c r="C327" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D327">
         <v>16220250</v>
@@ -7132,7 +7135,7 @@
         <v>330</v>
       </c>
       <c r="C328" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D328">
         <v>16407679</v>
@@ -7149,7 +7152,7 @@
         <v>331</v>
       </c>
       <c r="C329" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D329">
         <v>16600830</v>
@@ -7166,7 +7169,7 @@
         <v>332</v>
       </c>
       <c r="C330" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D330">
         <v>16810019</v>
@@ -7183,7 +7186,7 @@
         <v>333</v>
       </c>
       <c r="C331" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D331">
         <v>17055759</v>
@@ -7200,7 +7203,7 @@
         <v>334</v>
       </c>
       <c r="C332" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D332">
         <v>17294836</v>
@@ -7217,7 +7220,7 @@
         <v>335</v>
       </c>
       <c r="C333" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D333">
         <v>17545869</v>
@@ -7234,7 +7237,7 @@
         <v>336</v>
       </c>
       <c r="C334" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D334">
         <v>17737484</v>
@@ -7251,7 +7254,7 @@
         <v>337</v>
       </c>
       <c r="C335" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D335">
         <v>17925033</v>
@@ -7268,7 +7271,7 @@
         <v>338</v>
       </c>
       <c r="C336" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D336">
         <v>18123641</v>
@@ -7285,7 +7288,7 @@
         <v>339</v>
       </c>
       <c r="C337" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D337">
         <v>18320881</v>
@@ -7302,7 +7305,7 @@
         <v>340</v>
       </c>
       <c r="C338" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D338">
         <v>18549642</v>
@@ -7319,7 +7322,7 @@
         <v>341</v>
       </c>
       <c r="C339" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D339">
         <v>18742803</v>
@@ -7336,7 +7339,7 @@
         <v>342</v>
       </c>
       <c r="C340" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D340">
         <v>18839532</v>
@@ -7353,7 +7356,7 @@
         <v>343</v>
       </c>
       <c r="C341" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D341">
         <v>19066376</v>
@@ -7370,7 +7373,7 @@
         <v>344</v>
       </c>
       <c r="C342" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D342">
         <v>19222064</v>
@@ -7387,7 +7390,7 @@
         <v>345</v>
       </c>
       <c r="C343" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D343">
         <v>19396237</v>
@@ -7404,7 +7407,7 @@
         <v>346</v>
       </c>
       <c r="C344" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D344">
         <v>19595117</v>
@@ -7421,7 +7424,7 @@
         <v>347</v>
       </c>
       <c r="C345" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D345">
         <v>19827133</v>
@@ -7438,7 +7441,7 @@
         <v>348</v>
       </c>
       <c r="C346" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D346">
         <v>20061049</v>
@@ -7455,7 +7458,7 @@
         <v>349</v>
       </c>
       <c r="C347" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D347">
         <v>20213393</v>
@@ -7472,7 +7475,7 @@
         <v>350</v>
       </c>
       <c r="C348" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D348">
         <v>20513675</v>
@@ -7489,7 +7492,7 @@
         <v>351</v>
       </c>
       <c r="C349" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D349">
         <v>20722231</v>
@@ -7506,7 +7509,7 @@
         <v>352</v>
       </c>
       <c r="C350" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D350">
         <v>20906021</v>
@@ -7523,7 +7526,7 @@
         <v>353</v>
       </c>
       <c r="C351" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D351">
         <v>21139547</v>
@@ -7540,7 +7543,7 @@
         <v>354</v>
       </c>
       <c r="C352" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D352">
         <v>21393464</v>
@@ -7557,7 +7560,7 @@
         <v>355</v>
       </c>
       <c r="C353" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D353">
         <v>21670202</v>
@@ -7574,7 +7577,7 @@
         <v>356</v>
       </c>
       <c r="C354" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D354">
         <v>21962246</v>
@@ -7591,7 +7594,7 @@
         <v>357</v>
       </c>
       <c r="C355" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D355">
         <v>22224220</v>
@@ -7608,7 +7611,7 @@
         <v>358</v>
       </c>
       <c r="C356" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D356">
         <v>22437501</v>
@@ -7625,7 +7628,7 @@
         <v>359</v>
       </c>
       <c r="C357" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D357">
         <v>22651464</v>
@@ -7642,7 +7645,7 @@
         <v>360</v>
       </c>
       <c r="C358" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D358">
         <v>22877702</v>
@@ -7659,7 +7662,7 @@
         <v>361</v>
       </c>
       <c r="C359" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D359">
         <v>23107573</v>
@@ -7676,7 +7679,7 @@
         <v>362</v>
       </c>
       <c r="C360" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D360">
         <v>23342548</v>
@@ -7693,7 +7696,7 @@
         <v>363</v>
       </c>
       <c r="C361" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D361">
         <v>23583255</v>
@@ -7710,7 +7713,7 @@
         <v>364</v>
       </c>
       <c r="C362" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D362">
         <v>23784019</v>
@@ -7727,7 +7730,7 @@
         <v>365</v>
       </c>
       <c r="C363" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D363">
         <v>23961423</v>
@@ -7744,7 +7747,7 @@
         <v>366</v>
       </c>
       <c r="C364" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D364">
         <v>24104028</v>
@@ -7761,7 +7764,7 @@
         <v>367</v>
       </c>
       <c r="C365" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D365">
         <v>24281012</v>
@@ -7778,7 +7781,7 @@
         <v>368</v>
       </c>
       <c r="C366" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D366">
         <v>24463591</v>
@@ -7795,7 +7798,7 @@
         <v>369</v>
       </c>
       <c r="C367" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D367">
         <v>24656646</v>
@@ -7812,7 +7815,7 @@
         <v>370</v>
       </c>
       <c r="C368" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D368">
         <v>24846678</v>
@@ -7829,7 +7832,7 @@
         <v>371</v>
       </c>
       <c r="C369" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D369">
         <v>25016816</v>
@@ -7846,7 +7849,7 @@
         <v>372</v>
       </c>
       <c r="C370" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D370">
         <v>25147891</v>
@@ -7863,7 +7866,7 @@
         <v>373</v>
       </c>
       <c r="C371" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D371">
         <v>25298986</v>
@@ -7880,7 +7883,7 @@
         <v>374</v>
       </c>
       <c r="C372" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D372">
         <v>25445583</v>
@@ -7897,7 +7900,7 @@
         <v>375</v>
       </c>
       <c r="C373" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D373">
         <v>25598061</v>
@@ -7914,7 +7917,7 @@
         <v>376</v>
       </c>
       <c r="C374" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D374">
         <v>25766681</v>
@@ -7931,7 +7934,7 @@
         <v>377</v>
       </c>
       <c r="C375" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D375">
         <v>25932794</v>
@@ -7948,7 +7951,7 @@
         <v>378</v>
       </c>
       <c r="C376" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D376">
         <v>26074885</v>
@@ -7965,7 +7968,7 @@
         <v>379</v>
       </c>
       <c r="C377" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D377">
         <v>26186781</v>
@@ -7982,7 +7985,7 @@
         <v>380</v>
       </c>
       <c r="C378" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D378">
         <v>26321120</v>
@@ -7999,7 +8002,7 @@
         <v>381</v>
       </c>
       <c r="C379" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D379">
         <v>26435557</v>
@@ -8016,7 +8019,7 @@
         <v>382</v>
       </c>
       <c r="C380" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D380">
         <v>26557026</v>
@@ -8033,7 +8036,7 @@
         <v>383</v>
       </c>
       <c r="C381" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D381">
         <v>26680214</v>
@@ -8050,7 +8053,7 @@
         <v>384</v>
       </c>
       <c r="C382" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D382">
         <v>26813772</v>
@@ -8067,7 +8070,7 @@
         <v>385</v>
       </c>
       <c r="C383" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D383">
         <v>26917787</v>
@@ -8084,7 +8087,7 @@
         <v>386</v>
       </c>
       <c r="C384" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D384">
         <v>27007368</v>
@@ -8101,7 +8104,7 @@
         <v>387</v>
       </c>
       <c r="C385" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D385">
         <v>27097095</v>
@@ -8118,7 +8121,7 @@
         <v>388</v>
       </c>
       <c r="C386" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D386">
         <v>27192455</v>
@@ -8135,7 +8138,7 @@
         <v>389</v>
       </c>
       <c r="C387" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D387">
         <v>27287159</v>
@@ -8152,7 +8155,7 @@
         <v>390</v>
       </c>
       <c r="C388" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D388">
         <v>27392512</v>
@@ -8169,7 +8172,7 @@
         <v>391</v>
       </c>
       <c r="C389" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D389">
         <v>27492023</v>
@@ -8186,7 +8189,7 @@
         <v>392</v>
       </c>
       <c r="C390" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D390">
         <v>27575344</v>
@@ -8203,7 +8206,7 @@
         <v>393</v>
       </c>
       <c r="C391" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D391">
         <v>27640282</v>
@@ -8220,7 +8223,7 @@
         <v>394</v>
       </c>
       <c r="C392" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D392">
         <v>27694226</v>
@@ -8237,13 +8240,30 @@
         <v>395</v>
       </c>
       <c r="C393" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D393">
         <v>27756624</v>
       </c>
       <c r="E393">
         <v>488081</v>
+      </c>
+    </row>
+    <row r="394" spans="1:5">
+      <c r="A394" s="1">
+        <v>392</v>
+      </c>
+      <c r="B394" t="s">
+        <v>396</v>
+      </c>
+      <c r="C394" t="s">
+        <v>397</v>
+      </c>
+      <c r="D394">
+        <v>27826812</v>
+      </c>
+      <c r="E394">
+        <v>490540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated all of the graphics with plotly
</commit_message>
<xml_diff>
--- a/usa.xlsx
+++ b/usa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="399">
   <si>
     <t>date</t>
   </si>
@@ -1202,6 +1202,12 @@
   </si>
   <si>
     <t>2021-02-16</t>
+  </si>
+  <si>
+    <t>2021-02-17</t>
+  </si>
+  <si>
+    <t>2021-02-18</t>
   </si>
   <si>
     <t>united states of america</t>
@@ -1562,7 +1568,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E393"/>
+  <dimension ref="A1:E395"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1590,7 +1596,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1607,7 +1613,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1624,7 +1630,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1641,7 +1647,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1658,7 +1664,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1675,7 +1681,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1692,7 +1698,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1709,7 +1715,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -1726,7 +1732,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -1743,7 +1749,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D11">
         <v>8</v>
@@ -1760,7 +1766,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D12">
         <v>8</v>
@@ -1777,7 +1783,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -1794,7 +1800,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D14">
         <v>11</v>
@@ -1811,7 +1817,7 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -1828,7 +1834,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D16">
         <v>11</v>
@@ -1845,7 +1851,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D17">
         <v>12</v>
@@ -1862,7 +1868,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D18">
         <v>12</v>
@@ -1879,7 +1885,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D19">
         <v>12</v>
@@ -1896,7 +1902,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D20">
         <v>12</v>
@@ -1913,7 +1919,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D21">
         <v>12</v>
@@ -1930,7 +1936,7 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D22">
         <v>13</v>
@@ -1947,7 +1953,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D23">
         <v>13</v>
@@ -1964,7 +1970,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D24">
         <v>14</v>
@@ -1981,7 +1987,7 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D25">
         <v>14</v>
@@ -1998,7 +2004,7 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D26">
         <v>14</v>
@@ -2015,7 +2021,7 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D27">
         <v>14</v>
@@ -2032,7 +2038,7 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D28">
         <v>14</v>
@@ -2049,7 +2055,7 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D29">
         <v>14</v>
@@ -2066,7 +2072,7 @@
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D30">
         <v>14</v>
@@ -2083,7 +2089,7 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D31">
         <v>14</v>
@@ -2100,7 +2106,7 @@
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D32">
         <v>16</v>
@@ -2117,7 +2123,7 @@
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D33">
         <v>16</v>
@@ -2134,7 +2140,7 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D34">
         <v>16</v>
@@ -2151,7 +2157,7 @@
         <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D35">
         <v>16</v>
@@ -2168,7 +2174,7 @@
         <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D36">
         <v>16</v>
@@ -2185,7 +2191,7 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D37">
         <v>16</v>
@@ -2202,7 +2208,7 @@
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D38">
         <v>17</v>
@@ -2219,7 +2225,7 @@
         <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D39">
         <v>17</v>
@@ -2236,7 +2242,7 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D40">
         <v>25</v>
@@ -2253,7 +2259,7 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D41">
         <v>32</v>
@@ -2270,7 +2276,7 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D42">
         <v>55</v>
@@ -2287,7 +2293,7 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D43">
         <v>74</v>
@@ -2304,7 +2310,7 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D44">
         <v>107</v>
@@ -2321,7 +2327,7 @@
         <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D45">
         <v>184</v>
@@ -2338,7 +2344,7 @@
         <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D46">
         <v>237</v>
@@ -2355,7 +2361,7 @@
         <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D47">
         <v>403</v>
@@ -2372,7 +2378,7 @@
         <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D48">
         <v>519</v>
@@ -2389,7 +2395,7 @@
         <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D49">
         <v>594</v>
@@ -2406,7 +2412,7 @@
         <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D50">
         <v>782</v>
@@ -2423,7 +2429,7 @@
         <v>53</v>
       </c>
       <c r="C51" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D51">
         <v>1147</v>
@@ -2440,7 +2446,7 @@
         <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D52">
         <v>1586</v>
@@ -2457,7 +2463,7 @@
         <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D53">
         <v>2219</v>
@@ -2474,7 +2480,7 @@
         <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D54">
         <v>2978</v>
@@ -2491,7 +2497,7 @@
         <v>57</v>
       </c>
       <c r="C55" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D55">
         <v>3212</v>
@@ -2508,7 +2514,7 @@
         <v>58</v>
       </c>
       <c r="C56" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D56">
         <v>4679</v>
@@ -2525,7 +2531,7 @@
         <v>59</v>
       </c>
       <c r="C57" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D57">
         <v>6512</v>
@@ -2542,7 +2548,7 @@
         <v>60</v>
       </c>
       <c r="C58" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D58">
         <v>9169</v>
@@ -2559,7 +2565,7 @@
         <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D59">
         <v>13663</v>
@@ -2576,7 +2582,7 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D60">
         <v>20030</v>
@@ -2593,7 +2599,7 @@
         <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D61">
         <v>26025</v>
@@ -2610,7 +2616,7 @@
         <v>64</v>
       </c>
       <c r="C62" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D62">
         <v>34898</v>
@@ -2627,7 +2633,7 @@
         <v>65</v>
       </c>
       <c r="C63" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D63">
         <v>46136</v>
@@ -2644,7 +2650,7 @@
         <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D64">
         <v>56755</v>
@@ -2661,7 +2667,7 @@
         <v>67</v>
       </c>
       <c r="C65" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D65">
         <v>68837</v>
@@ -2678,7 +2684,7 @@
         <v>68</v>
       </c>
       <c r="C66" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D66">
         <v>86693</v>
@@ -2695,7 +2701,7 @@
         <v>69</v>
       </c>
       <c r="C67" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D67">
         <v>105383</v>
@@ -2712,7 +2718,7 @@
         <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D68">
         <v>125013</v>
@@ -2729,7 +2735,7 @@
         <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D69">
         <v>143912</v>
@@ -2746,7 +2752,7 @@
         <v>72</v>
       </c>
       <c r="C70" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D70">
         <v>165987</v>
@@ -2763,7 +2769,7 @@
         <v>73</v>
       </c>
       <c r="C71" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D71">
         <v>192301</v>
@@ -2780,7 +2786,7 @@
         <v>74</v>
       </c>
       <c r="C72" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D72">
         <v>224544</v>
@@ -2797,7 +2803,7 @@
         <v>75</v>
       </c>
       <c r="C73" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D73">
         <v>256779</v>
@@ -2814,7 +2820,7 @@
         <v>76</v>
       </c>
       <c r="C74" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D74">
         <v>289066</v>
@@ -2831,7 +2837,7 @@
         <v>77</v>
       </c>
       <c r="C75" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D75">
         <v>321482</v>
@@ -2848,7 +2854,7 @@
         <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D76">
         <v>351359</v>
@@ -2865,7 +2871,7 @@
         <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D77">
         <v>382740</v>
@@ -2882,7 +2888,7 @@
         <v>80</v>
       </c>
       <c r="C78" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D78">
         <v>413507</v>
@@ -2899,7 +2905,7 @@
         <v>81</v>
       </c>
       <c r="C79" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D79">
         <v>444699</v>
@@ -2916,7 +2922,7 @@
         <v>82</v>
       </c>
       <c r="C80" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D80">
         <v>480640</v>
@@ -2933,7 +2939,7 @@
         <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D81">
         <v>515055</v>
@@ -2950,7 +2956,7 @@
         <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D82">
         <v>544185</v>
@@ -2967,7 +2973,7 @@
         <v>85</v>
       </c>
       <c r="C83" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D83">
         <v>571440</v>
@@ -2984,7 +2990,7 @@
         <v>86</v>
       </c>
       <c r="C84" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D84">
         <v>598370</v>
@@ -3001,7 +3007,7 @@
         <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D85">
         <v>627151</v>
@@ -3018,7 +3024,7 @@
         <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D86">
         <v>652591</v>
@@ -3035,7 +3041,7 @@
         <v>89</v>
       </c>
       <c r="C87" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D87">
         <v>682626</v>
@@ -3052,7 +3058,7 @@
         <v>90</v>
       </c>
       <c r="C88" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D88">
         <v>715656</v>
@@ -3069,7 +3075,7 @@
         <v>91</v>
       </c>
       <c r="C89" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D89">
         <v>743588</v>
@@ -3086,7 +3092,7 @@
         <v>92</v>
       </c>
       <c r="C90" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D90">
         <v>769684</v>
@@ -3103,7 +3109,7 @@
         <v>93</v>
       </c>
       <c r="C91" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D91">
         <v>799512</v>
@@ -3120,7 +3126,7 @@
         <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D92">
         <v>825429</v>
@@ -3137,7 +3143,7 @@
         <v>95</v>
       </c>
       <c r="C93" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D93">
         <v>854288</v>
@@ -3154,7 +3160,7 @@
         <v>96</v>
       </c>
       <c r="C94" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D94">
         <v>887858</v>
@@ -3171,7 +3177,7 @@
         <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D95">
         <v>920185</v>
@@ -3188,7 +3194,7 @@
         <v>98</v>
       </c>
       <c r="C96" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D96">
         <v>950580</v>
@@ -3205,7 +3211,7 @@
         <v>99</v>
       </c>
       <c r="C97" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D97">
         <v>977081</v>
@@ -3222,7 +3228,7 @@
         <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D98">
         <v>1000784</v>
@@ -3239,7 +3245,7 @@
         <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D99">
         <v>1025361</v>
@@ -3256,7 +3262,7 @@
         <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D100">
         <v>1051799</v>
@@ -3273,7 +3279,7 @@
         <v>103</v>
       </c>
       <c r="C101" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D101">
         <v>1081019</v>
@@ -3290,7 +3296,7 @@
         <v>104</v>
       </c>
       <c r="C102" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D102">
         <v>1115945</v>
@@ -3307,7 +3313,7 @@
         <v>105</v>
       </c>
       <c r="C103" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D103">
         <v>1143295</v>
@@ -3324,7 +3330,7 @@
         <v>106</v>
       </c>
       <c r="C104" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D104">
         <v>1167592</v>
@@ -3341,7 +3347,7 @@
         <v>107</v>
       </c>
       <c r="C105" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D105">
         <v>1191677</v>
@@ -3358,7 +3364,7 @@
         <v>108</v>
       </c>
       <c r="C106" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D106">
         <v>1216208</v>
@@ -3375,7 +3381,7 @@
         <v>109</v>
       </c>
       <c r="C107" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D107">
         <v>1240767</v>
@@ -3392,7 +3398,7 @@
         <v>110</v>
       </c>
       <c r="C108" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D108">
         <v>1268179</v>
@@ -3409,7 +3415,7 @@
         <v>111</v>
       </c>
       <c r="C109" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D109">
         <v>1295017</v>
@@ -3426,7 +3432,7 @@
         <v>112</v>
       </c>
       <c r="C110" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D110">
         <v>1320153</v>
@@ -3443,7 +3449,7 @@
         <v>113</v>
       </c>
       <c r="C111" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D111">
         <v>1339020</v>
@@ -3460,7 +3466,7 @@
         <v>114</v>
       </c>
       <c r="C112" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D112">
         <v>1358291</v>
@@ -3477,7 +3483,7 @@
         <v>115</v>
       </c>
       <c r="C113" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D113">
         <v>1381238</v>
@@ -3494,7 +3500,7 @@
         <v>116</v>
       </c>
       <c r="C114" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D114">
         <v>1401646</v>
@@ -3511,7 +3517,7 @@
         <v>117</v>
       </c>
       <c r="C115" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D115">
         <v>1428464</v>
@@ -3528,7 +3534,7 @@
         <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D116">
         <v>1453211</v>
@@ -3545,7 +3551,7 @@
         <v>119</v>
       </c>
       <c r="C117" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D117">
         <v>1477370</v>
@@ -3562,7 +3568,7 @@
         <v>120</v>
       </c>
       <c r="C118" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D118">
         <v>1495733</v>
@@ -3579,7 +3585,7 @@
         <v>121</v>
       </c>
       <c r="C119" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D119">
         <v>1518123</v>
@@ -3596,7 +3602,7 @@
         <v>122</v>
       </c>
       <c r="C120" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D120">
         <v>1539130</v>
@@ -3613,7 +3619,7 @@
         <v>123</v>
       </c>
       <c r="C121" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D121">
         <v>1561827</v>
@@ -3630,7 +3636,7 @@
         <v>124</v>
       </c>
       <c r="C122" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D122">
         <v>1587593</v>
@@ -3647,7 +3653,7 @@
         <v>125</v>
       </c>
       <c r="C123" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D123">
         <v>1611249</v>
@@ -3664,7 +3670,7 @@
         <v>126</v>
       </c>
       <c r="C124" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D124">
         <v>1632361</v>
@@ -3681,7 +3687,7 @@
         <v>127</v>
       </c>
       <c r="C125" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D125">
         <v>1652428</v>
@@ -3698,7 +3704,7 @@
         <v>128</v>
       </c>
       <c r="C126" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D126">
         <v>1671100</v>
@@ -3715,7 +3721,7 @@
         <v>129</v>
       </c>
       <c r="C127" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D127">
         <v>1690750</v>
@@ -3732,7 +3738,7 @@
         <v>130</v>
       </c>
       <c r="C128" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D128">
         <v>1709299</v>
@@ -3749,7 +3755,7 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D129">
         <v>1731621</v>
@@ -3766,7 +3772,7 @@
         <v>132</v>
       </c>
       <c r="C130" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D130">
         <v>1756093</v>
@@ -3783,7 +3789,7 @@
         <v>133</v>
       </c>
       <c r="C131" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D131">
         <v>1779726</v>
@@ -3800,7 +3806,7 @@
         <v>134</v>
       </c>
       <c r="C132" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D132">
         <v>1798713</v>
@@ -3817,7 +3823,7 @@
         <v>135</v>
       </c>
       <c r="C133" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D133">
         <v>1816148</v>
@@ -3834,7 +3840,7 @@
         <v>136</v>
       </c>
       <c r="C134" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D134">
         <v>1837651</v>
@@ -3851,7 +3857,7 @@
         <v>137</v>
       </c>
       <c r="C135" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D135">
         <v>1857495</v>
@@ -3868,7 +3874,7 @@
         <v>138</v>
       </c>
       <c r="C136" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D136">
         <v>1879144</v>
@@ -3885,7 +3891,7 @@
         <v>139</v>
       </c>
       <c r="C137" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D137">
         <v>1904544</v>
@@ -3902,7 +3908,7 @@
         <v>140</v>
       </c>
       <c r="C138" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D138">
         <v>1925704</v>
@@ -3919,7 +3925,7 @@
         <v>141</v>
       </c>
       <c r="C139" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D139">
         <v>1943620</v>
@@ -3936,7 +3942,7 @@
         <v>142</v>
       </c>
       <c r="C140" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D140">
         <v>1961257</v>
@@ -3953,7 +3959,7 @@
         <v>143</v>
       </c>
       <c r="C141" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D141">
         <v>1979639</v>
@@ -3970,7 +3976,7 @@
         <v>144</v>
       </c>
       <c r="C142" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D142">
         <v>2000749</v>
@@ -3987,7 +3993,7 @@
         <v>145</v>
       </c>
       <c r="C143" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D143">
         <v>2023881</v>
@@ -4004,7 +4010,7 @@
         <v>146</v>
       </c>
       <c r="C144" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D144">
         <v>2048746</v>
@@ -4021,7 +4027,7 @@
         <v>147</v>
       </c>
       <c r="C145" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D145">
         <v>2073954</v>
@@ -4038,7 +4044,7 @@
         <v>148</v>
       </c>
       <c r="C146" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D146">
         <v>2092902</v>
@@ -4055,7 +4061,7 @@
         <v>149</v>
       </c>
       <c r="C147" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D147">
         <v>2112721</v>
@@ -4072,7 +4078,7 @@
         <v>150</v>
       </c>
       <c r="C148" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D148">
         <v>2136391</v>
@@ -4089,7 +4095,7 @@
         <v>151</v>
       </c>
       <c r="C149" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D149">
         <v>2163449</v>
@@ -4106,7 +4112,7 @@
         <v>152</v>
       </c>
       <c r="C150" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D150">
         <v>2191971</v>
@@ -4123,7 +4129,7 @@
         <v>153</v>
       </c>
       <c r="C151" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D151">
         <v>2223531</v>
@@ -4140,7 +4146,7 @@
         <v>154</v>
       </c>
       <c r="C152" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D152">
         <v>2255800</v>
@@ -4157,7 +4163,7 @@
         <v>155</v>
       </c>
       <c r="C153" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D153">
         <v>2280946</v>
@@ -4174,7 +4180,7 @@
         <v>156</v>
       </c>
       <c r="C154" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D154">
         <v>2313093</v>
@@ -4191,7 +4197,7 @@
         <v>157</v>
       </c>
       <c r="C155" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D155">
         <v>2350156</v>
@@ -4208,7 +4214,7 @@
         <v>158</v>
       </c>
       <c r="C156" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D156">
         <v>2386014</v>
@@ -4225,7 +4231,7 @@
         <v>159</v>
       </c>
       <c r="C157" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D157">
         <v>2426329</v>
@@ -4242,7 +4248,7 @@
         <v>160</v>
       </c>
       <c r="C158" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D158">
         <v>2472311</v>
@@ -4259,7 +4265,7 @@
         <v>161</v>
       </c>
       <c r="C159" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D159">
         <v>2513651</v>
@@ -4276,7 +4282,7 @@
         <v>162</v>
       </c>
       <c r="C160" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D160">
         <v>2554376</v>
@@ -4293,7 +4299,7 @@
         <v>163</v>
       </c>
       <c r="C161" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D161">
         <v>2595655</v>
@@ -4310,7 +4316,7 @@
         <v>164</v>
       </c>
       <c r="C162" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D162">
         <v>2642081</v>
@@ -4327,7 +4333,7 @@
         <v>165</v>
       </c>
       <c r="C163" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D163">
         <v>2693890</v>
@@ -4344,7 +4350,7 @@
         <v>166</v>
       </c>
       <c r="C164" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D164">
         <v>2750517</v>
@@ -4361,7 +4367,7 @@
         <v>167</v>
       </c>
       <c r="C165" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D165">
         <v>2801874</v>
@@ -4378,7 +4384,7 @@
         <v>168</v>
       </c>
       <c r="C166" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D166">
         <v>2847553</v>
@@ -4395,7 +4401,7 @@
         <v>169</v>
       </c>
       <c r="C167" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D167">
         <v>2898322</v>
@@ -4412,7 +4418,7 @@
         <v>170</v>
       </c>
       <c r="C168" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D168">
         <v>2941394</v>
@@ -4429,7 +4435,7 @@
         <v>171</v>
       </c>
       <c r="C169" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D169">
         <v>3002036</v>
@@ -4446,7 +4452,7 @@
         <v>172</v>
       </c>
       <c r="C170" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D170">
         <v>3062146</v>
@@ -4463,7 +4469,7 @@
         <v>173</v>
       </c>
       <c r="C171" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D171">
         <v>3124633</v>
@@ -4480,7 +4486,7 @@
         <v>174</v>
       </c>
       <c r="C172" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D172">
         <v>3192672</v>
@@ -4497,7 +4503,7 @@
         <v>175</v>
       </c>
       <c r="C173" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D173">
         <v>3252687</v>
@@ -4514,7 +4520,7 @@
         <v>176</v>
       </c>
       <c r="C174" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D174">
         <v>3311137</v>
@@ -4531,7 +4537,7 @@
         <v>177</v>
       </c>
       <c r="C175" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D175">
         <v>3370026</v>
@@ -4548,7 +4554,7 @@
         <v>178</v>
       </c>
       <c r="C176" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D176">
         <v>3438038</v>
@@ -4565,7 +4571,7 @@
         <v>179</v>
       </c>
       <c r="C177" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D177">
         <v>3506145</v>
@@ -4582,7 +4588,7 @@
         <v>180</v>
       </c>
       <c r="C178" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D178">
         <v>3581954</v>
@@ -4599,7 +4605,7 @@
         <v>181</v>
       </c>
       <c r="C179" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D179">
         <v>3654203</v>
@@ -4616,7 +4622,7 @@
         <v>182</v>
       </c>
       <c r="C180" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D180">
         <v>3716740</v>
@@ -4633,7 +4639,7 @@
         <v>183</v>
       </c>
       <c r="C181" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D181">
         <v>3777211</v>
@@ -4650,7 +4656,7 @@
         <v>184</v>
       </c>
       <c r="C182" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D182">
         <v>3839293</v>
@@ -4667,7 +4673,7 @@
         <v>185</v>
       </c>
       <c r="C183" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D183">
         <v>3903780</v>
@@ -4684,7 +4690,7 @@
         <v>186</v>
       </c>
       <c r="C184" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D184">
         <v>3974341</v>
@@ -4701,7 +4707,7 @@
         <v>187</v>
       </c>
       <c r="C185" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D185">
         <v>4042769</v>
@@ -4718,7 +4724,7 @@
         <v>188</v>
       </c>
       <c r="C186" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D186">
         <v>4116070</v>
@@ -4735,7 +4741,7 @@
         <v>189</v>
       </c>
       <c r="C187" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D187">
         <v>4180969</v>
@@ -4752,7 +4758,7 @@
         <v>190</v>
       </c>
       <c r="C188" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D188">
         <v>4235816</v>
@@ -4769,7 +4775,7 @@
         <v>191</v>
       </c>
       <c r="C189" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D189">
         <v>4292554</v>
@@ -4786,7 +4792,7 @@
         <v>192</v>
       </c>
       <c r="C190" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D190">
         <v>4359003</v>
@@ -4803,7 +4809,7 @@
         <v>193</v>
       </c>
       <c r="C191" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D191">
         <v>4430816</v>
@@ -4820,7 +4826,7 @@
         <v>194</v>
       </c>
       <c r="C192" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D192">
         <v>4498234</v>
@@ -4837,7 +4843,7 @@
         <v>195</v>
       </c>
       <c r="C193" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D193">
         <v>4566931</v>
@@ -4854,7 +4860,7 @@
         <v>196</v>
       </c>
       <c r="C194" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D194">
         <v>4623105</v>
@@ -4871,7 +4877,7 @@
         <v>197</v>
       </c>
       <c r="C195" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D195">
         <v>4668652</v>
@@ -4888,7 +4894,7 @@
         <v>198</v>
       </c>
       <c r="C196" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D196">
         <v>4714173</v>
@@ -4905,7 +4911,7 @@
         <v>199</v>
       </c>
       <c r="C197" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D197">
         <v>4772945</v>
@@ -4922,7 +4928,7 @@
         <v>200</v>
       </c>
       <c r="C198" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D198">
         <v>4827393</v>
@@ -4939,7 +4945,7 @@
         <v>201</v>
       </c>
       <c r="C199" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D199">
         <v>4886727</v>
@@ -4956,7 +4962,7 @@
         <v>202</v>
       </c>
       <c r="C200" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D200">
         <v>4945996</v>
@@ -4973,7 +4979,7 @@
         <v>203</v>
       </c>
       <c r="C201" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D201">
         <v>5000107</v>
@@ -4990,7 +4996,7 @@
         <v>204</v>
       </c>
       <c r="C202" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D202">
         <v>5045855</v>
@@ -5007,7 +5013,7 @@
         <v>205</v>
       </c>
       <c r="C203" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D203">
         <v>5093475</v>
@@ -5024,7 +5030,7 @@
         <v>206</v>
       </c>
       <c r="C204" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D204">
         <v>5141430</v>
@@ -5041,7 +5047,7 @@
         <v>207</v>
       </c>
       <c r="C205" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D205">
         <v>5197413</v>
@@ -5058,7 +5064,7 @@
         <v>208</v>
       </c>
       <c r="C206" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D206">
         <v>5248690</v>
@@ -5075,7 +5081,7 @@
         <v>209</v>
       </c>
       <c r="C207" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D207">
         <v>5314012</v>
@@ -5092,7 +5098,7 @@
         <v>210</v>
       </c>
       <c r="C208" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D208">
         <v>5360914</v>
@@ -5109,7 +5115,7 @@
         <v>211</v>
       </c>
       <c r="C209" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D209">
         <v>5400103</v>
@@ -5126,7 +5132,7 @@
         <v>212</v>
       </c>
       <c r="C210" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D210">
         <v>5436757</v>
@@ -5143,7 +5149,7 @@
         <v>213</v>
       </c>
       <c r="C211" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D211">
         <v>5481755</v>
@@ -5160,7 +5166,7 @@
         <v>214</v>
       </c>
       <c r="C212" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D212">
         <v>5529102</v>
@@ -5177,7 +5183,7 @@
         <v>215</v>
       </c>
       <c r="C213" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D213">
         <v>5572890</v>
@@ -5194,7 +5200,7 @@
         <v>216</v>
       </c>
       <c r="C214" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D214">
         <v>5621596</v>
@@ -5211,7 +5217,7 @@
         <v>217</v>
       </c>
       <c r="C215" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D215">
         <v>5664641</v>
@@ -5228,7 +5234,7 @@
         <v>218</v>
       </c>
       <c r="C216" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D216">
         <v>5698902</v>
@@ -5245,7 +5251,7 @@
         <v>219</v>
       </c>
       <c r="C217" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D217">
         <v>5735502</v>
@@ -5262,7 +5268,7 @@
         <v>220</v>
       </c>
       <c r="C218" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D218">
         <v>5775618</v>
@@ -5279,7 +5285,7 @@
         <v>221</v>
       </c>
       <c r="C219" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D219">
         <v>5820908</v>
@@ -5296,7 +5302,7 @@
         <v>222</v>
       </c>
       <c r="C220" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D220">
         <v>5866093</v>
@@ -5313,7 +5319,7 @@
         <v>223</v>
       </c>
       <c r="C221" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D221">
         <v>5913046</v>
@@ -5330,7 +5336,7 @@
         <v>224</v>
       </c>
       <c r="C222" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D222">
         <v>5955722</v>
@@ -5347,7 +5353,7 @@
         <v>225</v>
       </c>
       <c r="C223" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D223">
         <v>5990118</v>
@@ -5364,7 +5370,7 @@
         <v>226</v>
       </c>
       <c r="C224" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D224">
         <v>6025593</v>
@@ -5381,7 +5387,7 @@
         <v>227</v>
       </c>
       <c r="C225" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D225">
         <v>6067260</v>
@@ -5398,7 +5404,7 @@
         <v>228</v>
       </c>
       <c r="C226" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D226">
         <v>6108200</v>
@@ -5415,7 +5421,7 @@
         <v>229</v>
       </c>
       <c r="C227" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D227">
         <v>6152285</v>
@@ -5432,7 +5438,7 @@
         <v>230</v>
       </c>
       <c r="C228" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D228">
         <v>6202700</v>
@@ -5449,7 +5455,7 @@
         <v>231</v>
       </c>
       <c r="C229" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D229">
         <v>6245682</v>
@@ -5466,7 +5472,7 @@
         <v>232</v>
       </c>
       <c r="C230" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D230">
         <v>6276981</v>
@@ -5483,7 +5489,7 @@
         <v>233</v>
       </c>
       <c r="C231" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D231">
         <v>6300449</v>
@@ -5500,7 +5506,7 @@
         <v>234</v>
       </c>
       <c r="C232" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D232">
         <v>6327884</v>
@@ -5517,7 +5523,7 @@
         <v>235</v>
       </c>
       <c r="C233" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D233">
         <v>6361638</v>
@@ -5534,7 +5540,7 @@
         <v>236</v>
       </c>
       <c r="C234" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D234">
         <v>6397758</v>
@@ -5551,7 +5557,7 @@
         <v>237</v>
       </c>
       <c r="C235" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D235">
         <v>6445407</v>
@@ -5568,7 +5574,7 @@
         <v>238</v>
       </c>
       <c r="C236" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D236">
         <v>6486484</v>
@@ -5585,7 +5591,7 @@
         <v>239</v>
       </c>
       <c r="C237" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D237">
         <v>6520750</v>
@@ -5602,7 +5608,7 @@
         <v>240</v>
       </c>
       <c r="C238" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D238">
         <v>6555127</v>
@@ -5619,7 +5625,7 @@
         <v>241</v>
       </c>
       <c r="C239" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D239">
         <v>6594554</v>
@@ -5636,7 +5642,7 @@
         <v>242</v>
       </c>
       <c r="C240" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D240">
         <v>6633389</v>
@@ -5653,7 +5659,7 @@
         <v>243</v>
       </c>
       <c r="C241" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D241">
         <v>6678579</v>
@@ -5670,7 +5676,7 @@
         <v>244</v>
       </c>
       <c r="C242" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D242">
         <v>6727725</v>
@@ -5687,7 +5693,7 @@
         <v>245</v>
       </c>
       <c r="C243" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D243">
         <v>6769847</v>
@@ -5704,7 +5710,7 @@
         <v>246</v>
       </c>
       <c r="C244" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D244">
         <v>6808147</v>
@@ -5721,7 +5727,7 @@
         <v>247</v>
       </c>
       <c r="C245" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D245">
         <v>6860061</v>
@@ -5738,7 +5744,7 @@
         <v>248</v>
       </c>
       <c r="C246" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D246">
         <v>6899723</v>
@@ -5755,7 +5761,7 @@
         <v>249</v>
       </c>
       <c r="C247" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D247">
         <v>6938731</v>
@@ -5772,7 +5778,7 @@
         <v>250</v>
       </c>
       <c r="C248" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D248">
         <v>6985760</v>
@@ -5789,7 +5795,7 @@
         <v>251</v>
       </c>
       <c r="C249" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D249">
         <v>7033944</v>
@@ -5806,7 +5812,7 @@
         <v>252</v>
       </c>
       <c r="C250" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D250">
         <v>7078562</v>
@@ -5823,7 +5829,7 @@
         <v>253</v>
       </c>
       <c r="C251" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D251">
         <v>7116078</v>
@@ -5840,7 +5846,7 @@
         <v>254</v>
       </c>
       <c r="C252" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D252">
         <v>7149281</v>
@@ -5857,7 +5863,7 @@
         <v>255</v>
       </c>
       <c r="C253" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D253">
         <v>7192498</v>
@@ -5874,7 +5880,7 @@
         <v>256</v>
       </c>
       <c r="C254" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D254">
         <v>7231832</v>
@@ -5891,7 +5897,7 @@
         <v>257</v>
       </c>
       <c r="C255" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D255">
         <v>7277418</v>
@@ -5908,7 +5914,7 @@
         <v>258</v>
       </c>
       <c r="C256" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D256">
         <v>7332238</v>
@@ -5925,7 +5931,7 @@
         <v>259</v>
       </c>
       <c r="C257" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D257">
         <v>7380797</v>
@@ -5942,7 +5948,7 @@
         <v>260</v>
       </c>
       <c r="C258" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D258">
         <v>7416539</v>
@@ -5959,7 +5965,7 @@
         <v>261</v>
       </c>
       <c r="C259" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D259">
         <v>7455962</v>
@@ -5976,7 +5982,7 @@
         <v>262</v>
       </c>
       <c r="C260" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D260">
         <v>7501009</v>
@@ -5993,7 +5999,7 @@
         <v>263</v>
       </c>
       <c r="C261" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D261">
         <v>7551949</v>
@@ -6010,7 +6016,7 @@
         <v>264</v>
       </c>
       <c r="C262" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D262">
         <v>7610451</v>
@@ -6027,7 +6033,7 @@
         <v>265</v>
       </c>
       <c r="C263" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D263">
         <v>7666716</v>
@@ -6044,7 +6050,7 @@
         <v>266</v>
       </c>
       <c r="C264" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D264">
         <v>7721622</v>
@@ -6061,7 +6067,7 @@
         <v>267</v>
       </c>
       <c r="C265" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D265">
         <v>7767500</v>
@@ -6078,7 +6084,7 @@
         <v>268</v>
       </c>
       <c r="C266" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D266">
         <v>7809362</v>
@@ -6095,7 +6101,7 @@
         <v>269</v>
       </c>
       <c r="C267" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D267">
         <v>7861469</v>
@@ -6112,7 +6118,7 @@
         <v>270</v>
       </c>
       <c r="C268" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D268">
         <v>7921089</v>
@@ -6129,7 +6135,7 @@
         <v>271</v>
       </c>
       <c r="C269" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D269">
         <v>7985864</v>
@@ -6146,7 +6152,7 @@
         <v>272</v>
       </c>
       <c r="C270" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D270">
         <v>8054907</v>
@@ -6163,7 +6169,7 @@
         <v>273</v>
       </c>
       <c r="C271" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D271">
         <v>8111563</v>
@@ -6180,7 +6186,7 @@
         <v>274</v>
       </c>
       <c r="C272" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D272">
         <v>8160870</v>
@@ -6197,7 +6203,7 @@
         <v>275</v>
       </c>
       <c r="C273" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D273">
         <v>8228585</v>
@@ -6214,7 +6220,7 @@
         <v>276</v>
       </c>
       <c r="C274" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D274">
         <v>8290408</v>
@@ -6231,7 +6237,7 @@
         <v>277</v>
       </c>
       <c r="C275" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D275">
         <v>8353581</v>
@@ -6248,7 +6254,7 @@
         <v>278</v>
       </c>
       <c r="C276" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D276">
         <v>8429792</v>
@@ -6265,7 +6271,7 @@
         <v>279</v>
       </c>
       <c r="C277" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D277">
         <v>8511514</v>
@@ -6282,7 +6288,7 @@
         <v>280</v>
       </c>
       <c r="C278" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D278">
         <v>8594218</v>
@@ -6299,7 +6305,7 @@
         <v>281</v>
       </c>
       <c r="C279" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D279">
         <v>8656238</v>
@@ -6316,7 +6322,7 @@
         <v>282</v>
       </c>
       <c r="C280" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D280">
         <v>8723553</v>
@@ -6333,7 +6339,7 @@
         <v>283</v>
       </c>
       <c r="C281" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D281">
         <v>8800136</v>
@@ -6350,7 +6356,7 @@
         <v>284</v>
       </c>
       <c r="C282" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D282">
         <v>8879326</v>
@@ -6367,7 +6373,7 @@
         <v>285</v>
       </c>
       <c r="C283" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D283">
         <v>8970125</v>
@@ -6384,7 +6390,7 @@
         <v>286</v>
       </c>
       <c r="C284" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D284">
         <v>9069103</v>
@@ -6401,7 +6407,7 @@
         <v>287</v>
       </c>
       <c r="C285" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D285">
         <v>9158771</v>
@@ -6418,7 +6424,7 @@
         <v>288</v>
       </c>
       <c r="C286" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D286">
         <v>9263564</v>
@@ -6435,7 +6441,7 @@
         <v>289</v>
       </c>
       <c r="C287" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D287">
         <v>9348673</v>
@@ -6452,7 +6458,7 @@
         <v>290</v>
       </c>
       <c r="C288" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D288">
         <v>9475593</v>
@@ -6469,7 +6475,7 @@
         <v>291</v>
       </c>
       <c r="C289" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D289">
         <v>9579978</v>
@@ -6486,7 +6492,7 @@
         <v>292</v>
       </c>
       <c r="C290" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D290">
         <v>9709076</v>
@@ -6503,7 +6509,7 @@
         <v>293</v>
       </c>
       <c r="C291" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D291">
         <v>9836826</v>
@@ -6520,7 +6526,7 @@
         <v>294</v>
       </c>
       <c r="C292" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D292">
         <v>9964034</v>
@@ -6537,7 +6543,7 @@
         <v>295</v>
       </c>
       <c r="C293" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D293">
         <v>10079115</v>
@@ -6554,7 +6560,7 @@
         <v>296</v>
       </c>
       <c r="C294" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D294">
         <v>10199575</v>
@@ -6571,7 +6577,7 @@
         <v>297</v>
       </c>
       <c r="C295" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D295">
         <v>10339806</v>
@@ -6588,7 +6594,7 @@
         <v>298</v>
       </c>
       <c r="C296" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D296">
         <v>10486184</v>
@@ -6605,7 +6611,7 @@
         <v>299</v>
       </c>
       <c r="C297" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D297">
         <v>10650570</v>
@@ -6622,7 +6628,7 @@
         <v>300</v>
       </c>
       <c r="C298" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D298">
         <v>10830756</v>
@@ -6639,7 +6645,7 @@
         <v>301</v>
       </c>
       <c r="C299" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D299">
         <v>10998298</v>
@@ -6656,7 +6662,7 @@
         <v>302</v>
       </c>
       <c r="C300" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D300">
         <v>11134448</v>
@@ -6673,7 +6679,7 @@
         <v>303</v>
       </c>
       <c r="C301" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D301">
         <v>11296951</v>
@@ -6690,7 +6696,7 @@
         <v>304</v>
       </c>
       <c r="C302" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D302">
         <v>11460388</v>
@@ -6707,7 +6713,7 @@
         <v>305</v>
       </c>
       <c r="C303" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D303">
         <v>11633255</v>
@@ -6724,7 +6730,7 @@
         <v>306</v>
       </c>
       <c r="C304" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D304">
         <v>11824408</v>
@@ -6741,7 +6747,7 @@
         <v>307</v>
       </c>
       <c r="C305" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D305">
         <v>12022364</v>
@@ -6758,7 +6764,7 @@
         <v>308</v>
       </c>
       <c r="C306" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D306">
         <v>12201487</v>
@@ -6775,7 +6781,7 @@
         <v>309</v>
       </c>
       <c r="C307" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D307">
         <v>12348137</v>
@@ -6792,7 +6798,7 @@
         <v>310</v>
       </c>
       <c r="C308" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D308">
         <v>12522119</v>
@@ -6809,7 +6815,7 @@
         <v>311</v>
       </c>
       <c r="C309" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D309">
         <v>12697162</v>
@@ -6826,7 +6832,7 @@
         <v>312</v>
       </c>
       <c r="C310" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D310">
         <v>12879847</v>
@@ -6843,7 +6849,7 @@
         <v>313</v>
       </c>
       <c r="C311" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D311">
         <v>12991459</v>
@@ -6860,7 +6866,7 @@
         <v>314</v>
       </c>
       <c r="C312" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D312">
         <v>13199466</v>
@@ -6877,7 +6883,7 @@
         <v>315</v>
       </c>
       <c r="C313" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D313">
         <v>13354901</v>
@@ -6894,7 +6900,7 @@
         <v>316</v>
       </c>
       <c r="C314" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D314">
         <v>13494948</v>
@@ -6911,7 +6917,7 @@
         <v>317</v>
       </c>
       <c r="C315" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D315">
         <v>13655181</v>
@@ -6928,7 +6934,7 @@
         <v>318</v>
       </c>
       <c r="C316" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D316">
         <v>13842693</v>
@@ -6945,7 +6951,7 @@
         <v>319</v>
       </c>
       <c r="C317" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D317">
         <v>14044565</v>
@@ -6962,7 +6968,7 @@
         <v>320</v>
       </c>
       <c r="C318" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D318">
         <v>14266847</v>
@@ -6979,7 +6985,7 @@
         <v>321</v>
       </c>
       <c r="C319" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D319">
         <v>14498883</v>
@@ -6996,7 +7002,7 @@
         <v>322</v>
       </c>
       <c r="C320" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D320">
         <v>14713624</v>
@@ -7013,7 +7019,7 @@
         <v>323</v>
       </c>
       <c r="C321" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D321">
         <v>14894418</v>
@@ -7030,7 +7036,7 @@
         <v>324</v>
       </c>
       <c r="C322" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D322">
         <v>15089009</v>
@@ -7047,7 +7053,7 @@
         <v>325</v>
       </c>
       <c r="C323" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D323">
         <v>15312876</v>
@@ -7064,7 +7070,7 @@
         <v>326</v>
       </c>
       <c r="C324" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D324">
         <v>15534536</v>
@@ -7081,7 +7087,7 @@
         <v>327</v>
       </c>
       <c r="C325" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D325">
         <v>15765165</v>
@@ -7098,7 +7104,7 @@
         <v>328</v>
       </c>
       <c r="C326" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D326">
         <v>16003837</v>
@@ -7115,7 +7121,7 @@
         <v>329</v>
       </c>
       <c r="C327" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D327">
         <v>16220250</v>
@@ -7132,7 +7138,7 @@
         <v>330</v>
       </c>
       <c r="C328" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D328">
         <v>16407679</v>
@@ -7149,7 +7155,7 @@
         <v>331</v>
       </c>
       <c r="C329" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D329">
         <v>16600830</v>
@@ -7166,7 +7172,7 @@
         <v>332</v>
       </c>
       <c r="C330" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D330">
         <v>16810019</v>
@@ -7183,7 +7189,7 @@
         <v>333</v>
       </c>
       <c r="C331" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D331">
         <v>17055759</v>
@@ -7200,7 +7206,7 @@
         <v>334</v>
       </c>
       <c r="C332" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D332">
         <v>17294836</v>
@@ -7217,7 +7223,7 @@
         <v>335</v>
       </c>
       <c r="C333" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D333">
         <v>17545869</v>
@@ -7234,7 +7240,7 @@
         <v>336</v>
       </c>
       <c r="C334" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D334">
         <v>17737484</v>
@@ -7251,7 +7257,7 @@
         <v>337</v>
       </c>
       <c r="C335" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D335">
         <v>17925033</v>
@@ -7268,7 +7274,7 @@
         <v>338</v>
       </c>
       <c r="C336" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D336">
         <v>18123641</v>
@@ -7285,7 +7291,7 @@
         <v>339</v>
       </c>
       <c r="C337" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D337">
         <v>18320881</v>
@@ -7302,7 +7308,7 @@
         <v>340</v>
       </c>
       <c r="C338" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D338">
         <v>18549642</v>
@@ -7319,7 +7325,7 @@
         <v>341</v>
       </c>
       <c r="C339" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D339">
         <v>18742803</v>
@@ -7336,7 +7342,7 @@
         <v>342</v>
       </c>
       <c r="C340" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D340">
         <v>18839532</v>
@@ -7353,7 +7359,7 @@
         <v>343</v>
       </c>
       <c r="C341" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D341">
         <v>19066376</v>
@@ -7370,7 +7376,7 @@
         <v>344</v>
       </c>
       <c r="C342" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D342">
         <v>19222064</v>
@@ -7387,7 +7393,7 @@
         <v>345</v>
       </c>
       <c r="C343" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D343">
         <v>19396237</v>
@@ -7404,7 +7410,7 @@
         <v>346</v>
       </c>
       <c r="C344" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D344">
         <v>19595117</v>
@@ -7421,7 +7427,7 @@
         <v>347</v>
       </c>
       <c r="C345" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D345">
         <v>19827133</v>
@@ -7438,7 +7444,7 @@
         <v>348</v>
       </c>
       <c r="C346" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D346">
         <v>20061049</v>
@@ -7455,7 +7461,7 @@
         <v>349</v>
       </c>
       <c r="C347" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D347">
         <v>20213393</v>
@@ -7472,7 +7478,7 @@
         <v>350</v>
       </c>
       <c r="C348" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D348">
         <v>20513675</v>
@@ -7489,7 +7495,7 @@
         <v>351</v>
       </c>
       <c r="C349" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D349">
         <v>20722231</v>
@@ -7506,7 +7512,7 @@
         <v>352</v>
       </c>
       <c r="C350" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D350">
         <v>20906021</v>
@@ -7523,7 +7529,7 @@
         <v>353</v>
       </c>
       <c r="C351" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D351">
         <v>21139547</v>
@@ -7540,7 +7546,7 @@
         <v>354</v>
       </c>
       <c r="C352" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D352">
         <v>21393464</v>
@@ -7557,7 +7563,7 @@
         <v>355</v>
       </c>
       <c r="C353" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D353">
         <v>21670202</v>
@@ -7574,7 +7580,7 @@
         <v>356</v>
       </c>
       <c r="C354" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D354">
         <v>21962246</v>
@@ -7591,7 +7597,7 @@
         <v>357</v>
       </c>
       <c r="C355" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D355">
         <v>22224220</v>
@@ -7608,7 +7614,7 @@
         <v>358</v>
       </c>
       <c r="C356" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D356">
         <v>22437501</v>
@@ -7625,7 +7631,7 @@
         <v>359</v>
       </c>
       <c r="C357" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D357">
         <v>22651464</v>
@@ -7642,7 +7648,7 @@
         <v>360</v>
       </c>
       <c r="C358" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D358">
         <v>22877702</v>
@@ -7659,7 +7665,7 @@
         <v>361</v>
       </c>
       <c r="C359" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D359">
         <v>23107573</v>
@@ -7676,7 +7682,7 @@
         <v>362</v>
       </c>
       <c r="C360" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D360">
         <v>23342548</v>
@@ -7693,7 +7699,7 @@
         <v>363</v>
       </c>
       <c r="C361" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D361">
         <v>23583255</v>
@@ -7710,7 +7716,7 @@
         <v>364</v>
       </c>
       <c r="C362" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D362">
         <v>23784019</v>
@@ -7727,7 +7733,7 @@
         <v>365</v>
       </c>
       <c r="C363" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D363">
         <v>23961423</v>
@@ -7744,7 +7750,7 @@
         <v>366</v>
       </c>
       <c r="C364" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D364">
         <v>24104028</v>
@@ -7761,7 +7767,7 @@
         <v>367</v>
       </c>
       <c r="C365" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D365">
         <v>24281012</v>
@@ -7778,7 +7784,7 @@
         <v>368</v>
       </c>
       <c r="C366" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D366">
         <v>24463591</v>
@@ -7795,7 +7801,7 @@
         <v>369</v>
       </c>
       <c r="C367" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D367">
         <v>24656646</v>
@@ -7812,7 +7818,7 @@
         <v>370</v>
       </c>
       <c r="C368" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D368">
         <v>24846678</v>
@@ -7829,7 +7835,7 @@
         <v>371</v>
       </c>
       <c r="C369" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D369">
         <v>25016816</v>
@@ -7846,7 +7852,7 @@
         <v>372</v>
       </c>
       <c r="C370" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D370">
         <v>25147891</v>
@@ -7863,7 +7869,7 @@
         <v>373</v>
       </c>
       <c r="C371" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D371">
         <v>25298986</v>
@@ -7880,7 +7886,7 @@
         <v>374</v>
       </c>
       <c r="C372" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D372">
         <v>25445583</v>
@@ -7897,7 +7903,7 @@
         <v>375</v>
       </c>
       <c r="C373" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D373">
         <v>25598061</v>
@@ -7914,7 +7920,7 @@
         <v>376</v>
       </c>
       <c r="C374" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D374">
         <v>25766681</v>
@@ -7931,7 +7937,7 @@
         <v>377</v>
       </c>
       <c r="C375" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D375">
         <v>25932794</v>
@@ -7948,7 +7954,7 @@
         <v>378</v>
       </c>
       <c r="C376" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D376">
         <v>26074885</v>
@@ -7965,7 +7971,7 @@
         <v>379</v>
       </c>
       <c r="C377" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D377">
         <v>26186781</v>
@@ -7982,7 +7988,7 @@
         <v>380</v>
       </c>
       <c r="C378" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D378">
         <v>26321120</v>
@@ -7999,7 +8005,7 @@
         <v>381</v>
       </c>
       <c r="C379" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D379">
         <v>26435557</v>
@@ -8016,7 +8022,7 @@
         <v>382</v>
       </c>
       <c r="C380" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D380">
         <v>26557026</v>
@@ -8033,7 +8039,7 @@
         <v>383</v>
       </c>
       <c r="C381" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D381">
         <v>26680214</v>
@@ -8050,7 +8056,7 @@
         <v>384</v>
       </c>
       <c r="C382" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D382">
         <v>26813772</v>
@@ -8067,7 +8073,7 @@
         <v>385</v>
       </c>
       <c r="C383" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D383">
         <v>26917787</v>
@@ -8084,7 +8090,7 @@
         <v>386</v>
       </c>
       <c r="C384" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D384">
         <v>27007368</v>
@@ -8101,7 +8107,7 @@
         <v>387</v>
       </c>
       <c r="C385" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D385">
         <v>27097095</v>
@@ -8118,7 +8124,7 @@
         <v>388</v>
       </c>
       <c r="C386" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D386">
         <v>27192455</v>
@@ -8135,7 +8141,7 @@
         <v>389</v>
       </c>
       <c r="C387" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D387">
         <v>27287159</v>
@@ -8152,7 +8158,7 @@
         <v>390</v>
       </c>
       <c r="C388" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D388">
         <v>27392512</v>
@@ -8169,7 +8175,7 @@
         <v>391</v>
       </c>
       <c r="C389" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D389">
         <v>27492023</v>
@@ -8186,7 +8192,7 @@
         <v>392</v>
       </c>
       <c r="C390" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D390">
         <v>27575344</v>
@@ -8203,7 +8209,7 @@
         <v>393</v>
       </c>
       <c r="C391" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D391">
         <v>27640282</v>
@@ -8220,7 +8226,7 @@
         <v>394</v>
       </c>
       <c r="C392" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D392">
         <v>27694226</v>
@@ -8237,13 +8243,47 @@
         <v>395</v>
       </c>
       <c r="C393" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D393">
         <v>27756624</v>
       </c>
       <c r="E393">
         <v>488081</v>
+      </c>
+    </row>
+    <row r="394" spans="1:5">
+      <c r="A394" s="1">
+        <v>392</v>
+      </c>
+      <c r="B394" t="s">
+        <v>396</v>
+      </c>
+      <c r="C394" t="s">
+        <v>398</v>
+      </c>
+      <c r="D394">
+        <v>27826812</v>
+      </c>
+      <c r="E394">
+        <v>490540</v>
+      </c>
+    </row>
+    <row r="395" spans="1:5">
+      <c r="A395" s="1">
+        <v>393</v>
+      </c>
+      <c r="B395" t="s">
+        <v>397</v>
+      </c>
+      <c r="C395" t="s">
+        <v>398</v>
+      </c>
+      <c r="D395">
+        <v>27896040</v>
+      </c>
+      <c r="E395">
+        <v>493098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checked all segments, and created bitmap creation procedures for clustermaps
</commit_message>
<xml_diff>
--- a/usa.xlsx
+++ b/usa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="399">
   <si>
     <t>date</t>
   </si>
@@ -1205,6 +1205,9 @@
   </si>
   <si>
     <t>2021-02-17</t>
+  </si>
+  <si>
+    <t>2021-02-18</t>
   </si>
   <si>
     <t>united states of america</t>
@@ -1565,7 +1568,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E394"/>
+  <dimension ref="A1:E395"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1593,7 +1596,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1610,7 +1613,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1627,7 +1630,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1644,7 +1647,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1661,7 +1664,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1678,7 +1681,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1695,7 +1698,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1712,7 +1715,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -1729,7 +1732,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -1746,7 +1749,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D11">
         <v>8</v>
@@ -1763,7 +1766,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D12">
         <v>8</v>
@@ -1780,7 +1783,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -1797,7 +1800,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D14">
         <v>11</v>
@@ -1814,7 +1817,7 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -1831,7 +1834,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D16">
         <v>11</v>
@@ -1848,7 +1851,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D17">
         <v>12</v>
@@ -1865,7 +1868,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D18">
         <v>12</v>
@@ -1882,7 +1885,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D19">
         <v>12</v>
@@ -1899,7 +1902,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D20">
         <v>12</v>
@@ -1916,7 +1919,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D21">
         <v>12</v>
@@ -1933,7 +1936,7 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D22">
         <v>13</v>
@@ -1950,7 +1953,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D23">
         <v>13</v>
@@ -1967,7 +1970,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D24">
         <v>14</v>
@@ -1984,7 +1987,7 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D25">
         <v>14</v>
@@ -2001,7 +2004,7 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D26">
         <v>14</v>
@@ -2018,7 +2021,7 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D27">
         <v>14</v>
@@ -2035,7 +2038,7 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D28">
         <v>14</v>
@@ -2052,7 +2055,7 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D29">
         <v>14</v>
@@ -2069,7 +2072,7 @@
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D30">
         <v>14</v>
@@ -2086,7 +2089,7 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D31">
         <v>14</v>
@@ -2103,7 +2106,7 @@
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D32">
         <v>16</v>
@@ -2120,7 +2123,7 @@
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D33">
         <v>16</v>
@@ -2137,7 +2140,7 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D34">
         <v>16</v>
@@ -2154,7 +2157,7 @@
         <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D35">
         <v>16</v>
@@ -2171,7 +2174,7 @@
         <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D36">
         <v>16</v>
@@ -2188,7 +2191,7 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D37">
         <v>16</v>
@@ -2205,7 +2208,7 @@
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D38">
         <v>17</v>
@@ -2222,7 +2225,7 @@
         <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D39">
         <v>17</v>
@@ -2239,7 +2242,7 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D40">
         <v>25</v>
@@ -2256,7 +2259,7 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D41">
         <v>32</v>
@@ -2273,7 +2276,7 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D42">
         <v>55</v>
@@ -2290,7 +2293,7 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D43">
         <v>74</v>
@@ -2307,7 +2310,7 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D44">
         <v>107</v>
@@ -2324,7 +2327,7 @@
         <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D45">
         <v>184</v>
@@ -2341,7 +2344,7 @@
         <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D46">
         <v>237</v>
@@ -2358,7 +2361,7 @@
         <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D47">
         <v>403</v>
@@ -2375,7 +2378,7 @@
         <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D48">
         <v>519</v>
@@ -2392,7 +2395,7 @@
         <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D49">
         <v>594</v>
@@ -2409,7 +2412,7 @@
         <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D50">
         <v>782</v>
@@ -2426,7 +2429,7 @@
         <v>53</v>
       </c>
       <c r="C51" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D51">
         <v>1147</v>
@@ -2443,7 +2446,7 @@
         <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D52">
         <v>1586</v>
@@ -2460,7 +2463,7 @@
         <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D53">
         <v>2219</v>
@@ -2477,7 +2480,7 @@
         <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D54">
         <v>2978</v>
@@ -2494,7 +2497,7 @@
         <v>57</v>
       </c>
       <c r="C55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D55">
         <v>3212</v>
@@ -2511,7 +2514,7 @@
         <v>58</v>
       </c>
       <c r="C56" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D56">
         <v>4679</v>
@@ -2528,7 +2531,7 @@
         <v>59</v>
       </c>
       <c r="C57" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D57">
         <v>6512</v>
@@ -2545,7 +2548,7 @@
         <v>60</v>
       </c>
       <c r="C58" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D58">
         <v>9169</v>
@@ -2562,7 +2565,7 @@
         <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D59">
         <v>13663</v>
@@ -2579,7 +2582,7 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D60">
         <v>20030</v>
@@ -2596,7 +2599,7 @@
         <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D61">
         <v>26025</v>
@@ -2613,7 +2616,7 @@
         <v>64</v>
       </c>
       <c r="C62" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D62">
         <v>34898</v>
@@ -2630,7 +2633,7 @@
         <v>65</v>
       </c>
       <c r="C63" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D63">
         <v>46136</v>
@@ -2647,7 +2650,7 @@
         <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D64">
         <v>56755</v>
@@ -2664,7 +2667,7 @@
         <v>67</v>
       </c>
       <c r="C65" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D65">
         <v>68837</v>
@@ -2681,7 +2684,7 @@
         <v>68</v>
       </c>
       <c r="C66" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D66">
         <v>86693</v>
@@ -2698,7 +2701,7 @@
         <v>69</v>
       </c>
       <c r="C67" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D67">
         <v>105383</v>
@@ -2715,7 +2718,7 @@
         <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D68">
         <v>125013</v>
@@ -2732,7 +2735,7 @@
         <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D69">
         <v>143912</v>
@@ -2749,7 +2752,7 @@
         <v>72</v>
       </c>
       <c r="C70" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D70">
         <v>165987</v>
@@ -2766,7 +2769,7 @@
         <v>73</v>
       </c>
       <c r="C71" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D71">
         <v>192301</v>
@@ -2783,7 +2786,7 @@
         <v>74</v>
       </c>
       <c r="C72" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D72">
         <v>224544</v>
@@ -2800,7 +2803,7 @@
         <v>75</v>
       </c>
       <c r="C73" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D73">
         <v>256779</v>
@@ -2817,7 +2820,7 @@
         <v>76</v>
       </c>
       <c r="C74" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D74">
         <v>289066</v>
@@ -2834,7 +2837,7 @@
         <v>77</v>
       </c>
       <c r="C75" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D75">
         <v>321482</v>
@@ -2851,7 +2854,7 @@
         <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D76">
         <v>351359</v>
@@ -2868,7 +2871,7 @@
         <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D77">
         <v>382740</v>
@@ -2885,7 +2888,7 @@
         <v>80</v>
       </c>
       <c r="C78" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D78">
         <v>413507</v>
@@ -2902,7 +2905,7 @@
         <v>81</v>
       </c>
       <c r="C79" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D79">
         <v>444699</v>
@@ -2919,7 +2922,7 @@
         <v>82</v>
       </c>
       <c r="C80" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D80">
         <v>480640</v>
@@ -2936,7 +2939,7 @@
         <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D81">
         <v>515055</v>
@@ -2953,7 +2956,7 @@
         <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D82">
         <v>544185</v>
@@ -2970,7 +2973,7 @@
         <v>85</v>
       </c>
       <c r="C83" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D83">
         <v>571440</v>
@@ -2987,7 +2990,7 @@
         <v>86</v>
       </c>
       <c r="C84" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D84">
         <v>598370</v>
@@ -3004,7 +3007,7 @@
         <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D85">
         <v>627151</v>
@@ -3021,7 +3024,7 @@
         <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D86">
         <v>652591</v>
@@ -3038,7 +3041,7 @@
         <v>89</v>
       </c>
       <c r="C87" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D87">
         <v>682626</v>
@@ -3055,7 +3058,7 @@
         <v>90</v>
       </c>
       <c r="C88" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D88">
         <v>715656</v>
@@ -3072,7 +3075,7 @@
         <v>91</v>
       </c>
       <c r="C89" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D89">
         <v>743588</v>
@@ -3089,7 +3092,7 @@
         <v>92</v>
       </c>
       <c r="C90" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D90">
         <v>769684</v>
@@ -3106,7 +3109,7 @@
         <v>93</v>
       </c>
       <c r="C91" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D91">
         <v>799512</v>
@@ -3123,7 +3126,7 @@
         <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D92">
         <v>825429</v>
@@ -3140,7 +3143,7 @@
         <v>95</v>
       </c>
       <c r="C93" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D93">
         <v>854288</v>
@@ -3157,7 +3160,7 @@
         <v>96</v>
       </c>
       <c r="C94" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D94">
         <v>887858</v>
@@ -3174,7 +3177,7 @@
         <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D95">
         <v>920185</v>
@@ -3191,7 +3194,7 @@
         <v>98</v>
       </c>
       <c r="C96" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D96">
         <v>950580</v>
@@ -3208,7 +3211,7 @@
         <v>99</v>
       </c>
       <c r="C97" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D97">
         <v>977081</v>
@@ -3225,7 +3228,7 @@
         <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D98">
         <v>1000784</v>
@@ -3242,7 +3245,7 @@
         <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D99">
         <v>1025361</v>
@@ -3259,7 +3262,7 @@
         <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D100">
         <v>1051799</v>
@@ -3276,7 +3279,7 @@
         <v>103</v>
       </c>
       <c r="C101" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D101">
         <v>1081019</v>
@@ -3293,7 +3296,7 @@
         <v>104</v>
       </c>
       <c r="C102" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D102">
         <v>1115945</v>
@@ -3310,7 +3313,7 @@
         <v>105</v>
       </c>
       <c r="C103" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D103">
         <v>1143295</v>
@@ -3327,7 +3330,7 @@
         <v>106</v>
       </c>
       <c r="C104" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D104">
         <v>1167592</v>
@@ -3344,7 +3347,7 @@
         <v>107</v>
       </c>
       <c r="C105" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D105">
         <v>1191677</v>
@@ -3361,7 +3364,7 @@
         <v>108</v>
       </c>
       <c r="C106" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D106">
         <v>1216208</v>
@@ -3378,7 +3381,7 @@
         <v>109</v>
       </c>
       <c r="C107" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D107">
         <v>1240767</v>
@@ -3395,7 +3398,7 @@
         <v>110</v>
       </c>
       <c r="C108" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D108">
         <v>1268179</v>
@@ -3412,7 +3415,7 @@
         <v>111</v>
       </c>
       <c r="C109" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D109">
         <v>1295017</v>
@@ -3429,7 +3432,7 @@
         <v>112</v>
       </c>
       <c r="C110" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D110">
         <v>1320153</v>
@@ -3446,7 +3449,7 @@
         <v>113</v>
       </c>
       <c r="C111" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D111">
         <v>1339020</v>
@@ -3463,7 +3466,7 @@
         <v>114</v>
       </c>
       <c r="C112" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D112">
         <v>1358291</v>
@@ -3480,7 +3483,7 @@
         <v>115</v>
       </c>
       <c r="C113" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D113">
         <v>1381238</v>
@@ -3497,7 +3500,7 @@
         <v>116</v>
       </c>
       <c r="C114" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D114">
         <v>1401646</v>
@@ -3514,7 +3517,7 @@
         <v>117</v>
       </c>
       <c r="C115" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D115">
         <v>1428464</v>
@@ -3531,7 +3534,7 @@
         <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D116">
         <v>1453211</v>
@@ -3548,7 +3551,7 @@
         <v>119</v>
       </c>
       <c r="C117" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D117">
         <v>1477370</v>
@@ -3565,7 +3568,7 @@
         <v>120</v>
       </c>
       <c r="C118" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D118">
         <v>1495733</v>
@@ -3582,7 +3585,7 @@
         <v>121</v>
       </c>
       <c r="C119" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D119">
         <v>1518123</v>
@@ -3599,7 +3602,7 @@
         <v>122</v>
       </c>
       <c r="C120" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D120">
         <v>1539130</v>
@@ -3616,7 +3619,7 @@
         <v>123</v>
       </c>
       <c r="C121" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D121">
         <v>1561827</v>
@@ -3633,7 +3636,7 @@
         <v>124</v>
       </c>
       <c r="C122" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D122">
         <v>1587593</v>
@@ -3650,7 +3653,7 @@
         <v>125</v>
       </c>
       <c r="C123" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D123">
         <v>1611249</v>
@@ -3667,7 +3670,7 @@
         <v>126</v>
       </c>
       <c r="C124" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D124">
         <v>1632361</v>
@@ -3684,7 +3687,7 @@
         <v>127</v>
       </c>
       <c r="C125" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D125">
         <v>1652428</v>
@@ -3701,7 +3704,7 @@
         <v>128</v>
       </c>
       <c r="C126" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D126">
         <v>1671100</v>
@@ -3718,7 +3721,7 @@
         <v>129</v>
       </c>
       <c r="C127" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D127">
         <v>1690750</v>
@@ -3735,7 +3738,7 @@
         <v>130</v>
       </c>
       <c r="C128" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D128">
         <v>1709299</v>
@@ -3752,7 +3755,7 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D129">
         <v>1731621</v>
@@ -3769,7 +3772,7 @@
         <v>132</v>
       </c>
       <c r="C130" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D130">
         <v>1756093</v>
@@ -3786,7 +3789,7 @@
         <v>133</v>
       </c>
       <c r="C131" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D131">
         <v>1779726</v>
@@ -3803,7 +3806,7 @@
         <v>134</v>
       </c>
       <c r="C132" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D132">
         <v>1798713</v>
@@ -3820,7 +3823,7 @@
         <v>135</v>
       </c>
       <c r="C133" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D133">
         <v>1816148</v>
@@ -3837,7 +3840,7 @@
         <v>136</v>
       </c>
       <c r="C134" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D134">
         <v>1837651</v>
@@ -3854,7 +3857,7 @@
         <v>137</v>
       </c>
       <c r="C135" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D135">
         <v>1857495</v>
@@ -3871,7 +3874,7 @@
         <v>138</v>
       </c>
       <c r="C136" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D136">
         <v>1879144</v>
@@ -3888,7 +3891,7 @@
         <v>139</v>
       </c>
       <c r="C137" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D137">
         <v>1904544</v>
@@ -3905,7 +3908,7 @@
         <v>140</v>
       </c>
       <c r="C138" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D138">
         <v>1925704</v>
@@ -3922,7 +3925,7 @@
         <v>141</v>
       </c>
       <c r="C139" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D139">
         <v>1943620</v>
@@ -3939,7 +3942,7 @@
         <v>142</v>
       </c>
       <c r="C140" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D140">
         <v>1961257</v>
@@ -3956,7 +3959,7 @@
         <v>143</v>
       </c>
       <c r="C141" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D141">
         <v>1979639</v>
@@ -3973,7 +3976,7 @@
         <v>144</v>
       </c>
       <c r="C142" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D142">
         <v>2000749</v>
@@ -3990,7 +3993,7 @@
         <v>145</v>
       </c>
       <c r="C143" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D143">
         <v>2023881</v>
@@ -4007,7 +4010,7 @@
         <v>146</v>
       </c>
       <c r="C144" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D144">
         <v>2048746</v>
@@ -4024,7 +4027,7 @@
         <v>147</v>
       </c>
       <c r="C145" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D145">
         <v>2073954</v>
@@ -4041,7 +4044,7 @@
         <v>148</v>
       </c>
       <c r="C146" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D146">
         <v>2092902</v>
@@ -4058,7 +4061,7 @@
         <v>149</v>
       </c>
       <c r="C147" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D147">
         <v>2112721</v>
@@ -4075,7 +4078,7 @@
         <v>150</v>
       </c>
       <c r="C148" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D148">
         <v>2136391</v>
@@ -4092,7 +4095,7 @@
         <v>151</v>
       </c>
       <c r="C149" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D149">
         <v>2163449</v>
@@ -4109,7 +4112,7 @@
         <v>152</v>
       </c>
       <c r="C150" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D150">
         <v>2191971</v>
@@ -4126,7 +4129,7 @@
         <v>153</v>
       </c>
       <c r="C151" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D151">
         <v>2223531</v>
@@ -4143,7 +4146,7 @@
         <v>154</v>
       </c>
       <c r="C152" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D152">
         <v>2255800</v>
@@ -4160,7 +4163,7 @@
         <v>155</v>
       </c>
       <c r="C153" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D153">
         <v>2280946</v>
@@ -4177,7 +4180,7 @@
         <v>156</v>
       </c>
       <c r="C154" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D154">
         <v>2313093</v>
@@ -4194,7 +4197,7 @@
         <v>157</v>
       </c>
       <c r="C155" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D155">
         <v>2350156</v>
@@ -4211,7 +4214,7 @@
         <v>158</v>
       </c>
       <c r="C156" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D156">
         <v>2386014</v>
@@ -4228,7 +4231,7 @@
         <v>159</v>
       </c>
       <c r="C157" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D157">
         <v>2426329</v>
@@ -4245,7 +4248,7 @@
         <v>160</v>
       </c>
       <c r="C158" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D158">
         <v>2472311</v>
@@ -4262,7 +4265,7 @@
         <v>161</v>
       </c>
       <c r="C159" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D159">
         <v>2513651</v>
@@ -4279,7 +4282,7 @@
         <v>162</v>
       </c>
       <c r="C160" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D160">
         <v>2554376</v>
@@ -4296,7 +4299,7 @@
         <v>163</v>
       </c>
       <c r="C161" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D161">
         <v>2595655</v>
@@ -4313,7 +4316,7 @@
         <v>164</v>
       </c>
       <c r="C162" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D162">
         <v>2642081</v>
@@ -4330,7 +4333,7 @@
         <v>165</v>
       </c>
       <c r="C163" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D163">
         <v>2693890</v>
@@ -4347,7 +4350,7 @@
         <v>166</v>
       </c>
       <c r="C164" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D164">
         <v>2750517</v>
@@ -4364,7 +4367,7 @@
         <v>167</v>
       </c>
       <c r="C165" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D165">
         <v>2801874</v>
@@ -4381,7 +4384,7 @@
         <v>168</v>
       </c>
       <c r="C166" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D166">
         <v>2847553</v>
@@ -4398,7 +4401,7 @@
         <v>169</v>
       </c>
       <c r="C167" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D167">
         <v>2898322</v>
@@ -4415,7 +4418,7 @@
         <v>170</v>
       </c>
       <c r="C168" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D168">
         <v>2941394</v>
@@ -4432,7 +4435,7 @@
         <v>171</v>
       </c>
       <c r="C169" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D169">
         <v>3002036</v>
@@ -4449,7 +4452,7 @@
         <v>172</v>
       </c>
       <c r="C170" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D170">
         <v>3062146</v>
@@ -4466,7 +4469,7 @@
         <v>173</v>
       </c>
       <c r="C171" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D171">
         <v>3124633</v>
@@ -4483,7 +4486,7 @@
         <v>174</v>
       </c>
       <c r="C172" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D172">
         <v>3192672</v>
@@ -4500,7 +4503,7 @@
         <v>175</v>
       </c>
       <c r="C173" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D173">
         <v>3252687</v>
@@ -4517,7 +4520,7 @@
         <v>176</v>
       </c>
       <c r="C174" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D174">
         <v>3311137</v>
@@ -4534,7 +4537,7 @@
         <v>177</v>
       </c>
       <c r="C175" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D175">
         <v>3370026</v>
@@ -4551,7 +4554,7 @@
         <v>178</v>
       </c>
       <c r="C176" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D176">
         <v>3438038</v>
@@ -4568,7 +4571,7 @@
         <v>179</v>
       </c>
       <c r="C177" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D177">
         <v>3506145</v>
@@ -4585,7 +4588,7 @@
         <v>180</v>
       </c>
       <c r="C178" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D178">
         <v>3581954</v>
@@ -4602,7 +4605,7 @@
         <v>181</v>
       </c>
       <c r="C179" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D179">
         <v>3654203</v>
@@ -4619,7 +4622,7 @@
         <v>182</v>
       </c>
       <c r="C180" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D180">
         <v>3716740</v>
@@ -4636,7 +4639,7 @@
         <v>183</v>
       </c>
       <c r="C181" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D181">
         <v>3777211</v>
@@ -4653,7 +4656,7 @@
         <v>184</v>
       </c>
       <c r="C182" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D182">
         <v>3839293</v>
@@ -4670,7 +4673,7 @@
         <v>185</v>
       </c>
       <c r="C183" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D183">
         <v>3903780</v>
@@ -4687,7 +4690,7 @@
         <v>186</v>
       </c>
       <c r="C184" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D184">
         <v>3974341</v>
@@ -4704,7 +4707,7 @@
         <v>187</v>
       </c>
       <c r="C185" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D185">
         <v>4042769</v>
@@ -4721,7 +4724,7 @@
         <v>188</v>
       </c>
       <c r="C186" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D186">
         <v>4116070</v>
@@ -4738,7 +4741,7 @@
         <v>189</v>
       </c>
       <c r="C187" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D187">
         <v>4180969</v>
@@ -4755,7 +4758,7 @@
         <v>190</v>
       </c>
       <c r="C188" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D188">
         <v>4235816</v>
@@ -4772,7 +4775,7 @@
         <v>191</v>
       </c>
       <c r="C189" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D189">
         <v>4292554</v>
@@ -4789,7 +4792,7 @@
         <v>192</v>
       </c>
       <c r="C190" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D190">
         <v>4359003</v>
@@ -4806,7 +4809,7 @@
         <v>193</v>
       </c>
       <c r="C191" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D191">
         <v>4430816</v>
@@ -4823,7 +4826,7 @@
         <v>194</v>
       </c>
       <c r="C192" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D192">
         <v>4498234</v>
@@ -4840,7 +4843,7 @@
         <v>195</v>
       </c>
       <c r="C193" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D193">
         <v>4566931</v>
@@ -4857,7 +4860,7 @@
         <v>196</v>
       </c>
       <c r="C194" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D194">
         <v>4623105</v>
@@ -4874,7 +4877,7 @@
         <v>197</v>
       </c>
       <c r="C195" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D195">
         <v>4668652</v>
@@ -4891,7 +4894,7 @@
         <v>198</v>
       </c>
       <c r="C196" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D196">
         <v>4714173</v>
@@ -4908,7 +4911,7 @@
         <v>199</v>
       </c>
       <c r="C197" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D197">
         <v>4772945</v>
@@ -4925,7 +4928,7 @@
         <v>200</v>
       </c>
       <c r="C198" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D198">
         <v>4827393</v>
@@ -4942,7 +4945,7 @@
         <v>201</v>
       </c>
       <c r="C199" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D199">
         <v>4886727</v>
@@ -4959,7 +4962,7 @@
         <v>202</v>
       </c>
       <c r="C200" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D200">
         <v>4945996</v>
@@ -4976,7 +4979,7 @@
         <v>203</v>
       </c>
       <c r="C201" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D201">
         <v>5000107</v>
@@ -4993,7 +4996,7 @@
         <v>204</v>
       </c>
       <c r="C202" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D202">
         <v>5045855</v>
@@ -5010,7 +5013,7 @@
         <v>205</v>
       </c>
       <c r="C203" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D203">
         <v>5093475</v>
@@ -5027,7 +5030,7 @@
         <v>206</v>
       </c>
       <c r="C204" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D204">
         <v>5141430</v>
@@ -5044,7 +5047,7 @@
         <v>207</v>
       </c>
       <c r="C205" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D205">
         <v>5197413</v>
@@ -5061,7 +5064,7 @@
         <v>208</v>
       </c>
       <c r="C206" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D206">
         <v>5248690</v>
@@ -5078,7 +5081,7 @@
         <v>209</v>
       </c>
       <c r="C207" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D207">
         <v>5314012</v>
@@ -5095,7 +5098,7 @@
         <v>210</v>
       </c>
       <c r="C208" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D208">
         <v>5360914</v>
@@ -5112,7 +5115,7 @@
         <v>211</v>
       </c>
       <c r="C209" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D209">
         <v>5400103</v>
@@ -5129,7 +5132,7 @@
         <v>212</v>
       </c>
       <c r="C210" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D210">
         <v>5436757</v>
@@ -5146,7 +5149,7 @@
         <v>213</v>
       </c>
       <c r="C211" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D211">
         <v>5481755</v>
@@ -5163,7 +5166,7 @@
         <v>214</v>
       </c>
       <c r="C212" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D212">
         <v>5529102</v>
@@ -5180,7 +5183,7 @@
         <v>215</v>
       </c>
       <c r="C213" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D213">
         <v>5572890</v>
@@ -5197,7 +5200,7 @@
         <v>216</v>
       </c>
       <c r="C214" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D214">
         <v>5621596</v>
@@ -5214,7 +5217,7 @@
         <v>217</v>
       </c>
       <c r="C215" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D215">
         <v>5664641</v>
@@ -5231,7 +5234,7 @@
         <v>218</v>
       </c>
       <c r="C216" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D216">
         <v>5698902</v>
@@ -5248,7 +5251,7 @@
         <v>219</v>
       </c>
       <c r="C217" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D217">
         <v>5735502</v>
@@ -5265,7 +5268,7 @@
         <v>220</v>
       </c>
       <c r="C218" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D218">
         <v>5775618</v>
@@ -5282,7 +5285,7 @@
         <v>221</v>
       </c>
       <c r="C219" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D219">
         <v>5820908</v>
@@ -5299,7 +5302,7 @@
         <v>222</v>
       </c>
       <c r="C220" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D220">
         <v>5866093</v>
@@ -5316,7 +5319,7 @@
         <v>223</v>
       </c>
       <c r="C221" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D221">
         <v>5913046</v>
@@ -5333,7 +5336,7 @@
         <v>224</v>
       </c>
       <c r="C222" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D222">
         <v>5955722</v>
@@ -5350,7 +5353,7 @@
         <v>225</v>
       </c>
       <c r="C223" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D223">
         <v>5990118</v>
@@ -5367,7 +5370,7 @@
         <v>226</v>
       </c>
       <c r="C224" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D224">
         <v>6025593</v>
@@ -5384,7 +5387,7 @@
         <v>227</v>
       </c>
       <c r="C225" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D225">
         <v>6067260</v>
@@ -5401,7 +5404,7 @@
         <v>228</v>
       </c>
       <c r="C226" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D226">
         <v>6108200</v>
@@ -5418,7 +5421,7 @@
         <v>229</v>
       </c>
       <c r="C227" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D227">
         <v>6152285</v>
@@ -5435,7 +5438,7 @@
         <v>230</v>
       </c>
       <c r="C228" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D228">
         <v>6202700</v>
@@ -5452,7 +5455,7 @@
         <v>231</v>
       </c>
       <c r="C229" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D229">
         <v>6245682</v>
@@ -5469,7 +5472,7 @@
         <v>232</v>
       </c>
       <c r="C230" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D230">
         <v>6276981</v>
@@ -5486,7 +5489,7 @@
         <v>233</v>
       </c>
       <c r="C231" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D231">
         <v>6300449</v>
@@ -5503,7 +5506,7 @@
         <v>234</v>
       </c>
       <c r="C232" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D232">
         <v>6327884</v>
@@ -5520,7 +5523,7 @@
         <v>235</v>
       </c>
       <c r="C233" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D233">
         <v>6361638</v>
@@ -5537,7 +5540,7 @@
         <v>236</v>
       </c>
       <c r="C234" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D234">
         <v>6397758</v>
@@ -5554,7 +5557,7 @@
         <v>237</v>
       </c>
       <c r="C235" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D235">
         <v>6445407</v>
@@ -5571,7 +5574,7 @@
         <v>238</v>
       </c>
       <c r="C236" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D236">
         <v>6486484</v>
@@ -5588,7 +5591,7 @@
         <v>239</v>
       </c>
       <c r="C237" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D237">
         <v>6520750</v>
@@ -5605,7 +5608,7 @@
         <v>240</v>
       </c>
       <c r="C238" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D238">
         <v>6555127</v>
@@ -5622,7 +5625,7 @@
         <v>241</v>
       </c>
       <c r="C239" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D239">
         <v>6594554</v>
@@ -5639,7 +5642,7 @@
         <v>242</v>
       </c>
       <c r="C240" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D240">
         <v>6633389</v>
@@ -5656,7 +5659,7 @@
         <v>243</v>
       </c>
       <c r="C241" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D241">
         <v>6678579</v>
@@ -5673,7 +5676,7 @@
         <v>244</v>
       </c>
       <c r="C242" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D242">
         <v>6727725</v>
@@ -5690,7 +5693,7 @@
         <v>245</v>
       </c>
       <c r="C243" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D243">
         <v>6769847</v>
@@ -5707,7 +5710,7 @@
         <v>246</v>
       </c>
       <c r="C244" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D244">
         <v>6808147</v>
@@ -5724,7 +5727,7 @@
         <v>247</v>
       </c>
       <c r="C245" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D245">
         <v>6860061</v>
@@ -5741,7 +5744,7 @@
         <v>248</v>
       </c>
       <c r="C246" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D246">
         <v>6899723</v>
@@ -5758,7 +5761,7 @@
         <v>249</v>
       </c>
       <c r="C247" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D247">
         <v>6938731</v>
@@ -5775,7 +5778,7 @@
         <v>250</v>
       </c>
       <c r="C248" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D248">
         <v>6985760</v>
@@ -5792,7 +5795,7 @@
         <v>251</v>
       </c>
       <c r="C249" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D249">
         <v>7033944</v>
@@ -5809,7 +5812,7 @@
         <v>252</v>
       </c>
       <c r="C250" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D250">
         <v>7078562</v>
@@ -5826,7 +5829,7 @@
         <v>253</v>
       </c>
       <c r="C251" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D251">
         <v>7116078</v>
@@ -5843,7 +5846,7 @@
         <v>254</v>
       </c>
       <c r="C252" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D252">
         <v>7149281</v>
@@ -5860,7 +5863,7 @@
         <v>255</v>
       </c>
       <c r="C253" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D253">
         <v>7192498</v>
@@ -5877,7 +5880,7 @@
         <v>256</v>
       </c>
       <c r="C254" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D254">
         <v>7231832</v>
@@ -5894,7 +5897,7 @@
         <v>257</v>
       </c>
       <c r="C255" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D255">
         <v>7277418</v>
@@ -5911,7 +5914,7 @@
         <v>258</v>
       </c>
       <c r="C256" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D256">
         <v>7332238</v>
@@ -5928,7 +5931,7 @@
         <v>259</v>
       </c>
       <c r="C257" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D257">
         <v>7380797</v>
@@ -5945,7 +5948,7 @@
         <v>260</v>
       </c>
       <c r="C258" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D258">
         <v>7416539</v>
@@ -5962,7 +5965,7 @@
         <v>261</v>
       </c>
       <c r="C259" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D259">
         <v>7455962</v>
@@ -5979,7 +5982,7 @@
         <v>262</v>
       </c>
       <c r="C260" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D260">
         <v>7501009</v>
@@ -5996,7 +5999,7 @@
         <v>263</v>
       </c>
       <c r="C261" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D261">
         <v>7551949</v>
@@ -6013,7 +6016,7 @@
         <v>264</v>
       </c>
       <c r="C262" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D262">
         <v>7610451</v>
@@ -6030,7 +6033,7 @@
         <v>265</v>
       </c>
       <c r="C263" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D263">
         <v>7666716</v>
@@ -6047,7 +6050,7 @@
         <v>266</v>
       </c>
       <c r="C264" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D264">
         <v>7721622</v>
@@ -6064,7 +6067,7 @@
         <v>267</v>
       </c>
       <c r="C265" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D265">
         <v>7767500</v>
@@ -6081,7 +6084,7 @@
         <v>268</v>
       </c>
       <c r="C266" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D266">
         <v>7809362</v>
@@ -6098,7 +6101,7 @@
         <v>269</v>
       </c>
       <c r="C267" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D267">
         <v>7861469</v>
@@ -6115,7 +6118,7 @@
         <v>270</v>
       </c>
       <c r="C268" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D268">
         <v>7921089</v>
@@ -6132,7 +6135,7 @@
         <v>271</v>
       </c>
       <c r="C269" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D269">
         <v>7985864</v>
@@ -6149,7 +6152,7 @@
         <v>272</v>
       </c>
       <c r="C270" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D270">
         <v>8054907</v>
@@ -6166,7 +6169,7 @@
         <v>273</v>
       </c>
       <c r="C271" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D271">
         <v>8111563</v>
@@ -6183,7 +6186,7 @@
         <v>274</v>
       </c>
       <c r="C272" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D272">
         <v>8160870</v>
@@ -6200,7 +6203,7 @@
         <v>275</v>
       </c>
       <c r="C273" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D273">
         <v>8228585</v>
@@ -6217,7 +6220,7 @@
         <v>276</v>
       </c>
       <c r="C274" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D274">
         <v>8290408</v>
@@ -6234,7 +6237,7 @@
         <v>277</v>
       </c>
       <c r="C275" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D275">
         <v>8353581</v>
@@ -6251,7 +6254,7 @@
         <v>278</v>
       </c>
       <c r="C276" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D276">
         <v>8429792</v>
@@ -6268,7 +6271,7 @@
         <v>279</v>
       </c>
       <c r="C277" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D277">
         <v>8511514</v>
@@ -6285,7 +6288,7 @@
         <v>280</v>
       </c>
       <c r="C278" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D278">
         <v>8594218</v>
@@ -6302,7 +6305,7 @@
         <v>281</v>
       </c>
       <c r="C279" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D279">
         <v>8656238</v>
@@ -6319,7 +6322,7 @@
         <v>282</v>
       </c>
       <c r="C280" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D280">
         <v>8723553</v>
@@ -6336,7 +6339,7 @@
         <v>283</v>
       </c>
       <c r="C281" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D281">
         <v>8800136</v>
@@ -6353,7 +6356,7 @@
         <v>284</v>
       </c>
       <c r="C282" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D282">
         <v>8879326</v>
@@ -6370,7 +6373,7 @@
         <v>285</v>
       </c>
       <c r="C283" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D283">
         <v>8970125</v>
@@ -6387,7 +6390,7 @@
         <v>286</v>
       </c>
       <c r="C284" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D284">
         <v>9069103</v>
@@ -6404,7 +6407,7 @@
         <v>287</v>
       </c>
       <c r="C285" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D285">
         <v>9158771</v>
@@ -6421,10 +6424,10 @@
         <v>288</v>
       </c>
       <c r="C286" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D286">
-        <v>9263564</v>
+        <v>9263540</v>
       </c>
       <c r="E286">
         <v>232831</v>
@@ -6438,10 +6441,10 @@
         <v>289</v>
       </c>
       <c r="C287" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D287">
-        <v>9348673</v>
+        <v>9348641</v>
       </c>
       <c r="E287">
         <v>233407</v>
@@ -6455,10 +6458,10 @@
         <v>290</v>
       </c>
       <c r="C288" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D288">
-        <v>9475593</v>
+        <v>9475561</v>
       </c>
       <c r="E288">
         <v>234987</v>
@@ -6472,10 +6475,10 @@
         <v>291</v>
       </c>
       <c r="C289" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D289">
-        <v>9579978</v>
+        <v>9579953</v>
       </c>
       <c r="E289">
         <v>236111</v>
@@ -6489,10 +6492,10 @@
         <v>292</v>
       </c>
       <c r="C290" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D290">
-        <v>9709076</v>
+        <v>9709053</v>
       </c>
       <c r="E290">
         <v>237269</v>
@@ -6506,10 +6509,10 @@
         <v>293</v>
       </c>
       <c r="C291" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D291">
-        <v>9836826</v>
+        <v>9836805</v>
       </c>
       <c r="E291">
         <v>238503</v>
@@ -6523,10 +6526,10 @@
         <v>294</v>
       </c>
       <c r="C292" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D292">
-        <v>9964034</v>
+        <v>9964007</v>
       </c>
       <c r="E292">
         <v>239580</v>
@@ -6540,10 +6543,10 @@
         <v>295</v>
       </c>
       <c r="C293" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D293">
-        <v>10079115</v>
+        <v>10079085</v>
       </c>
       <c r="E293">
         <v>240151</v>
@@ -6557,10 +6560,10 @@
         <v>296</v>
       </c>
       <c r="C294" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D294">
-        <v>10199575</v>
+        <v>10199542</v>
       </c>
       <c r="E294">
         <v>240939</v>
@@ -6574,10 +6577,10 @@
         <v>297</v>
       </c>
       <c r="C295" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D295">
-        <v>10339806</v>
+        <v>10339769</v>
       </c>
       <c r="E295">
         <v>242362</v>
@@ -6591,10 +6594,10 @@
         <v>298</v>
       </c>
       <c r="C296" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D296">
-        <v>10486184</v>
+        <v>10486134</v>
       </c>
       <c r="E296">
         <v>243804</v>
@@ -6608,10 +6611,10 @@
         <v>299</v>
       </c>
       <c r="C297" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D297">
-        <v>10650570</v>
+        <v>10650509</v>
       </c>
       <c r="E297">
         <v>245015</v>
@@ -6625,10 +6628,10 @@
         <v>300</v>
       </c>
       <c r="C298" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D298">
-        <v>10830756</v>
+        <v>10830672</v>
       </c>
       <c r="E298">
         <v>246220</v>
@@ -6642,10 +6645,10 @@
         <v>301</v>
       </c>
       <c r="C299" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D299">
-        <v>10998298</v>
+        <v>10998189</v>
       </c>
       <c r="E299">
         <v>247561</v>
@@ -6659,10 +6662,10 @@
         <v>302</v>
       </c>
       <c r="C300" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D300">
-        <v>11134448</v>
+        <v>11134318</v>
       </c>
       <c r="E300">
         <v>248329</v>
@@ -6676,10 +6679,10 @@
         <v>303</v>
       </c>
       <c r="C301" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D301">
-        <v>11296951</v>
+        <v>11296818</v>
       </c>
       <c r="E301">
         <v>249174</v>
@@ -6693,10 +6696,10 @@
         <v>304</v>
       </c>
       <c r="C302" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D302">
-        <v>11460388</v>
+        <v>11460242</v>
       </c>
       <c r="E302">
         <v>250900</v>
@@ -6710,10 +6713,10 @@
         <v>305</v>
       </c>
       <c r="C303" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D303">
-        <v>11633255</v>
+        <v>11633088</v>
       </c>
       <c r="E303">
         <v>252838</v>
@@ -6727,10 +6730,10 @@
         <v>306</v>
       </c>
       <c r="C304" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D304">
-        <v>11824408</v>
+        <v>11824228</v>
       </c>
       <c r="E304">
         <v>254879</v>
@@ -6744,10 +6747,10 @@
         <v>307</v>
       </c>
       <c r="C305" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D305">
-        <v>12022364</v>
+        <v>12022158</v>
       </c>
       <c r="E305">
         <v>256836</v>
@@ -6761,10 +6764,10 @@
         <v>308</v>
       </c>
       <c r="C306" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D306">
-        <v>12201487</v>
+        <v>12201266</v>
       </c>
       <c r="E306">
         <v>258454</v>
@@ -6778,10 +6781,10 @@
         <v>309</v>
       </c>
       <c r="C307" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D307">
-        <v>12348137</v>
+        <v>12347905</v>
       </c>
       <c r="E307">
         <v>259481</v>
@@ -6795,10 +6798,10 @@
         <v>310</v>
       </c>
       <c r="C308" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D308">
-        <v>12522119</v>
+        <v>12521898</v>
       </c>
       <c r="E308">
         <v>260591</v>
@@ -6812,10 +6815,10 @@
         <v>311</v>
       </c>
       <c r="C309" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D309">
-        <v>12697162</v>
+        <v>12697001</v>
       </c>
       <c r="E309">
         <v>262730</v>
@@ -6829,10 +6832,10 @@
         <v>312</v>
       </c>
       <c r="C310" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D310">
-        <v>12879847</v>
+        <v>12879677</v>
       </c>
       <c r="E310">
         <v>265001</v>
@@ -6846,10 +6849,10 @@
         <v>313</v>
       </c>
       <c r="C311" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D311">
-        <v>12991459</v>
+        <v>12991818</v>
       </c>
       <c r="E311">
         <v>266385</v>
@@ -6863,10 +6866,10 @@
         <v>314</v>
       </c>
       <c r="C312" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D312">
-        <v>13199466</v>
+        <v>13199752</v>
       </c>
       <c r="E312">
         <v>267940</v>
@@ -6880,10 +6883,10 @@
         <v>315</v>
       </c>
       <c r="C313" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D313">
-        <v>13354901</v>
+        <v>13355018</v>
       </c>
       <c r="E313">
         <v>269303</v>
@@ -6897,10 +6900,10 @@
         <v>316</v>
       </c>
       <c r="C314" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D314">
-        <v>13494948</v>
+        <v>13495104</v>
       </c>
       <c r="E314">
         <v>270340</v>
@@ -6914,10 +6917,10 @@
         <v>317</v>
       </c>
       <c r="C315" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D315">
-        <v>13655181</v>
+        <v>13655220</v>
       </c>
       <c r="E315">
         <v>271710</v>
@@ -6931,10 +6934,10 @@
         <v>318</v>
       </c>
       <c r="C316" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D316">
-        <v>13842693</v>
+        <v>13842652</v>
       </c>
       <c r="E316">
         <v>274267</v>
@@ -6948,10 +6951,10 @@
         <v>319</v>
       </c>
       <c r="C317" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D317">
-        <v>14044565</v>
+        <v>14044625</v>
       </c>
       <c r="E317">
         <v>277087</v>
@@ -6965,10 +6968,10 @@
         <v>320</v>
       </c>
       <c r="C318" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D318">
-        <v>14266847</v>
+        <v>14267421</v>
       </c>
       <c r="E318">
         <v>280049</v>
@@ -6982,10 +6985,10 @@
         <v>321</v>
       </c>
       <c r="C319" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D319">
-        <v>14498883</v>
+        <v>14499637</v>
       </c>
       <c r="E319">
         <v>282725</v>
@@ -6999,10 +7002,10 @@
         <v>322</v>
       </c>
       <c r="C320" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D320">
-        <v>14713624</v>
+        <v>14714853</v>
       </c>
       <c r="E320">
         <v>285067</v>
@@ -7016,10 +7019,10 @@
         <v>323</v>
       </c>
       <c r="C321" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D321">
-        <v>14894418</v>
+        <v>14895691</v>
       </c>
       <c r="E321">
         <v>286408</v>
@@ -7033,10 +7036,10 @@
         <v>324</v>
       </c>
       <c r="C322" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D322">
-        <v>15089009</v>
+        <v>15089952</v>
       </c>
       <c r="E322">
         <v>288034</v>
@@ -7050,10 +7053,10 @@
         <v>325</v>
       </c>
       <c r="C323" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D323">
-        <v>15312876</v>
+        <v>15313819</v>
       </c>
       <c r="E323">
         <v>290668</v>
@@ -7067,10 +7070,10 @@
         <v>326</v>
       </c>
       <c r="C324" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D324">
-        <v>15534536</v>
+        <v>15535463</v>
       </c>
       <c r="E324">
         <v>293847</v>
@@ -7084,10 +7087,10 @@
         <v>327</v>
       </c>
       <c r="C325" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D325">
-        <v>15765165</v>
+        <v>15766130</v>
       </c>
       <c r="E325">
         <v>296830</v>
@@ -7101,10 +7104,10 @@
         <v>328</v>
       </c>
       <c r="C326" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D326">
-        <v>16003837</v>
+        <v>16004659</v>
       </c>
       <c r="E326">
         <v>300246</v>
@@ -7118,10 +7121,10 @@
         <v>329</v>
       </c>
       <c r="C327" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D327">
-        <v>16220250</v>
+        <v>16221125</v>
       </c>
       <c r="E327">
         <v>302698</v>
@@ -7135,10 +7138,10 @@
         <v>330</v>
       </c>
       <c r="C328" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D328">
-        <v>16407679</v>
+        <v>16408428</v>
       </c>
       <c r="E328">
         <v>304301</v>
@@ -7152,10 +7155,10 @@
         <v>331</v>
       </c>
       <c r="C329" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D329">
-        <v>16600830</v>
+        <v>16601499</v>
       </c>
       <c r="E329">
         <v>305998</v>
@@ -7169,10 +7172,10 @@
         <v>332</v>
       </c>
       <c r="C330" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D330">
-        <v>16810019</v>
+        <v>16810792</v>
       </c>
       <c r="E330">
         <v>309092</v>
@@ -7186,10 +7189,10 @@
         <v>333</v>
       </c>
       <c r="C331" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D331">
-        <v>17055759</v>
+        <v>17056440</v>
       </c>
       <c r="E331">
         <v>312813</v>
@@ -7203,10 +7206,10 @@
         <v>334</v>
       </c>
       <c r="C332" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D332">
-        <v>17294836</v>
+        <v>17295460</v>
       </c>
       <c r="E332">
         <v>316274</v>
@@ -7220,10 +7223,10 @@
         <v>335</v>
       </c>
       <c r="C333" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D333">
-        <v>17545869</v>
+        <v>17546621</v>
       </c>
       <c r="E333">
         <v>319223</v>
@@ -7237,10 +7240,10 @@
         <v>336</v>
       </c>
       <c r="C334" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D334">
-        <v>17737484</v>
+        <v>17738237</v>
       </c>
       <c r="E334">
         <v>321859</v>
@@ -7254,10 +7257,10 @@
         <v>337</v>
       </c>
       <c r="C335" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D335">
-        <v>17925033</v>
+        <v>17925587</v>
       </c>
       <c r="E335">
         <v>323557</v>
@@ -7271,10 +7274,10 @@
         <v>338</v>
       </c>
       <c r="C336" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D336">
-        <v>18123641</v>
+        <v>18123968</v>
       </c>
       <c r="E336">
         <v>325533</v>
@@ -7288,10 +7291,10 @@
         <v>339</v>
       </c>
       <c r="C337" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D337">
-        <v>18320881</v>
+        <v>18321157</v>
       </c>
       <c r="E337">
         <v>328921</v>
@@ -7305,10 +7308,10 @@
         <v>340</v>
       </c>
       <c r="C338" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D338">
-        <v>18549642</v>
+        <v>18550002</v>
       </c>
       <c r="E338">
         <v>332362</v>
@@ -7322,10 +7325,10 @@
         <v>341</v>
       </c>
       <c r="C339" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D339">
-        <v>18742803</v>
+        <v>18743916</v>
       </c>
       <c r="E339">
         <v>335248</v>
@@ -7339,10 +7342,10 @@
         <v>342</v>
       </c>
       <c r="C340" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D340">
-        <v>18839532</v>
+        <v>18841414</v>
       </c>
       <c r="E340">
         <v>336631</v>
@@ -7356,10 +7359,10 @@
         <v>343</v>
       </c>
       <c r="C341" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D341">
-        <v>19066376</v>
+        <v>19067574</v>
       </c>
       <c r="E341">
         <v>338497</v>
@@ -7373,10 +7376,10 @@
         <v>344</v>
       </c>
       <c r="C342" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D342">
-        <v>19222064</v>
+        <v>19222891</v>
       </c>
       <c r="E342">
         <v>339916</v>
@@ -7390,10 +7393,10 @@
         <v>345</v>
       </c>
       <c r="C343" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D343">
-        <v>19396237</v>
+        <v>19396787</v>
       </c>
       <c r="E343">
         <v>341944</v>
@@ -7407,10 +7410,10 @@
         <v>346</v>
       </c>
       <c r="C344" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D344">
-        <v>19595117</v>
+        <v>19595354</v>
       </c>
       <c r="E344">
         <v>345582</v>
@@ -7424,10 +7427,10 @@
         <v>347</v>
       </c>
       <c r="C345" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D345">
-        <v>19827133</v>
+        <v>19827770</v>
       </c>
       <c r="E345">
         <v>349326</v>
@@ -7441,10 +7444,10 @@
         <v>348</v>
       </c>
       <c r="C346" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D346">
-        <v>20061049</v>
+        <v>20061903</v>
       </c>
       <c r="E346">
         <v>352752</v>
@@ -7458,10 +7461,10 @@
         <v>349</v>
       </c>
       <c r="C347" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D347">
-        <v>20213393</v>
+        <v>20215297</v>
       </c>
       <c r="E347">
         <v>354862</v>
@@ -7475,10 +7478,10 @@
         <v>350</v>
       </c>
       <c r="C348" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D348">
-        <v>20513675</v>
+        <v>20515083</v>
       </c>
       <c r="E348">
         <v>357281</v>
@@ -7492,10 +7495,10 @@
         <v>351</v>
       </c>
       <c r="C349" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D349">
-        <v>20722231</v>
+        <v>20723157</v>
       </c>
       <c r="E349">
         <v>358645</v>
@@ -7509,10 +7512,10 @@
         <v>352</v>
       </c>
       <c r="C350" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D350">
-        <v>20906021</v>
+        <v>20906563</v>
       </c>
       <c r="E350">
         <v>360708</v>
@@ -7526,10 +7529,10 @@
         <v>353</v>
       </c>
       <c r="C351" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D351">
-        <v>21139547</v>
+        <v>21140217</v>
       </c>
       <c r="E351">
         <v>364312</v>
@@ -7543,10 +7546,10 @@
         <v>354</v>
       </c>
       <c r="C352" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D352">
-        <v>21393464</v>
+        <v>21394210</v>
       </c>
       <c r="E352">
         <v>368160</v>
@@ -7560,10 +7563,10 @@
         <v>355</v>
       </c>
       <c r="C353" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D353">
-        <v>21670202</v>
+        <v>21671278</v>
       </c>
       <c r="E353">
         <v>372065</v>
@@ -7577,10 +7580,10 @@
         <v>356</v>
       </c>
       <c r="C354" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D354">
-        <v>21962246</v>
+        <v>21963383</v>
       </c>
       <c r="E354">
         <v>376073</v>
@@ -7594,10 +7597,10 @@
         <v>357</v>
       </c>
       <c r="C355" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D355">
-        <v>22224220</v>
+        <v>22225720</v>
       </c>
       <c r="E355">
         <v>379318</v>
@@ -7611,10 +7614,10 @@
         <v>358</v>
       </c>
       <c r="C356" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D356">
-        <v>22437501</v>
+        <v>22438881</v>
       </c>
       <c r="E356">
         <v>381219</v>
@@ -7628,10 +7631,10 @@
         <v>359</v>
       </c>
       <c r="C357" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D357">
-        <v>22651464</v>
+        <v>22653070</v>
       </c>
       <c r="E357">
         <v>383241</v>
@@ -7645,10 +7648,10 @@
         <v>360</v>
       </c>
       <c r="C358" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D358">
-        <v>22877702</v>
+        <v>22879069</v>
       </c>
       <c r="E358">
         <v>387642</v>
@@ -7662,10 +7665,10 @@
         <v>361</v>
       </c>
       <c r="C359" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D359">
-        <v>23107573</v>
+        <v>23108826</v>
       </c>
       <c r="E359">
         <v>391601</v>
@@ -7679,10 +7682,10 @@
         <v>362</v>
       </c>
       <c r="C360" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D360">
-        <v>23342548</v>
+        <v>23343727</v>
       </c>
       <c r="E360">
         <v>395506</v>
@@ -7696,10 +7699,10 @@
         <v>363</v>
       </c>
       <c r="C361" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D361">
-        <v>23583255</v>
+        <v>23584671</v>
       </c>
       <c r="E361">
         <v>399312</v>
@@ -7713,10 +7716,10 @@
         <v>364</v>
       </c>
       <c r="C362" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D362">
-        <v>23784019</v>
+        <v>23785679</v>
       </c>
       <c r="E362">
         <v>402658</v>
@@ -7730,10 +7733,10 @@
         <v>365</v>
       </c>
       <c r="C363" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D363">
-        <v>23961423</v>
+        <v>23962788</v>
       </c>
       <c r="E363">
         <v>404447</v>
@@ -7747,10 +7750,10 @@
         <v>366</v>
       </c>
       <c r="C364" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D364">
-        <v>24104028</v>
+        <v>24105873</v>
       </c>
       <c r="E364">
         <v>405871</v>
@@ -7764,10 +7767,10 @@
         <v>367</v>
       </c>
       <c r="C365" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D365">
-        <v>24281012</v>
+        <v>24281531</v>
       </c>
       <c r="E365">
         <v>408569</v>
@@ -7781,10 +7784,10 @@
         <v>368</v>
       </c>
       <c r="C366" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D366">
-        <v>24463591</v>
+        <v>24464045</v>
       </c>
       <c r="E366">
         <v>412902</v>
@@ -7798,10 +7801,10 @@
         <v>369</v>
       </c>
       <c r="C367" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D367">
-        <v>24656646</v>
+        <v>24656940</v>
       </c>
       <c r="E367">
         <v>417032</v>
@@ -7815,10 +7818,10 @@
         <v>370</v>
       </c>
       <c r="C368" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D368">
-        <v>24846678</v>
+        <v>24846933</v>
       </c>
       <c r="E368">
         <v>420788</v>
@@ -7832,10 +7835,10 @@
         <v>371</v>
       </c>
       <c r="C369" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D369">
-        <v>25016816</v>
+        <v>25017235</v>
       </c>
       <c r="E369">
         <v>424071</v>
@@ -7849,10 +7852,10 @@
         <v>372</v>
       </c>
       <c r="C370" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D370">
-        <v>25147891</v>
+        <v>25148046</v>
       </c>
       <c r="E370">
         <v>425892</v>
@@ -7866,10 +7869,10 @@
         <v>373</v>
       </c>
       <c r="C371" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D371">
-        <v>25298986</v>
+        <v>25299108</v>
       </c>
       <c r="E371">
         <v>427825</v>
@@ -7883,10 +7886,10 @@
         <v>374</v>
       </c>
       <c r="C372" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D372">
-        <v>25445583</v>
+        <v>25445778</v>
       </c>
       <c r="E372">
         <v>431816</v>
@@ -7900,10 +7903,10 @@
         <v>375</v>
       </c>
       <c r="C373" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D373">
-        <v>25598061</v>
+        <v>25598384</v>
       </c>
       <c r="E373">
         <v>435729</v>
@@ -7917,10 +7920,10 @@
         <v>376</v>
       </c>
       <c r="C374" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D374">
-        <v>25766681</v>
+        <v>25767014</v>
       </c>
       <c r="E374">
         <v>439700</v>
@@ -7934,10 +7937,10 @@
         <v>377</v>
       </c>
       <c r="C375" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D375">
-        <v>25932794</v>
+        <v>25933090</v>
       </c>
       <c r="E375">
         <v>443271</v>
@@ -7951,10 +7954,10 @@
         <v>378</v>
       </c>
       <c r="C376" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D376">
-        <v>26074885</v>
+        <v>26075178</v>
       </c>
       <c r="E376">
         <v>445983</v>
@@ -7968,10 +7971,10 @@
         <v>379</v>
       </c>
       <c r="C377" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D377">
-        <v>26186781</v>
+        <v>26187035</v>
       </c>
       <c r="E377">
         <v>447772</v>
@@ -7985,10 +7988,10 @@
         <v>380</v>
       </c>
       <c r="C378" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D378">
-        <v>26321120</v>
+        <v>26321351</v>
       </c>
       <c r="E378">
         <v>449786</v>
@@ -8002,10 +8005,10 @@
         <v>381</v>
       </c>
       <c r="C379" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D379">
-        <v>26435557</v>
+        <v>26436155</v>
       </c>
       <c r="E379">
         <v>453217</v>
@@ -8019,10 +8022,10 @@
         <v>382</v>
       </c>
       <c r="C380" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D380">
-        <v>26557026</v>
+        <v>26557346</v>
       </c>
       <c r="E380">
         <v>457043</v>
@@ -8036,10 +8039,10 @@
         <v>383</v>
       </c>
       <c r="C381" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D381">
-        <v>26680214</v>
+        <v>26680589</v>
       </c>
       <c r="E381">
         <v>460763</v>
@@ -8053,10 +8056,10 @@
         <v>384</v>
       </c>
       <c r="C382" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D382">
-        <v>26813772</v>
+        <v>26814096</v>
       </c>
       <c r="E382">
         <v>464344</v>
@@ -8070,10 +8073,10 @@
         <v>385</v>
       </c>
       <c r="C383" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D383">
-        <v>26917787</v>
+        <v>26917986</v>
       </c>
       <c r="E383">
         <v>466890</v>
@@ -8087,10 +8090,10 @@
         <v>386</v>
       </c>
       <c r="C384" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D384">
-        <v>27007368</v>
+        <v>27007586</v>
       </c>
       <c r="E384">
         <v>468204</v>
@@ -8104,10 +8107,10 @@
         <v>387</v>
       </c>
       <c r="C385" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D385">
-        <v>27097095</v>
+        <v>27097493</v>
       </c>
       <c r="E385">
         <v>469786</v>
@@ -8121,10 +8124,10 @@
         <v>388</v>
       </c>
       <c r="C386" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D386">
-        <v>27192455</v>
+        <v>27192663</v>
       </c>
       <c r="E386">
         <v>472818</v>
@@ -8138,10 +8141,10 @@
         <v>389</v>
       </c>
       <c r="C387" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D387">
-        <v>27287159</v>
+        <v>27287431</v>
       </c>
       <c r="E387">
         <v>476100</v>
@@ -8155,10 +8158,10 @@
         <v>390</v>
       </c>
       <c r="C388" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D388">
-        <v>27392512</v>
+        <v>27392829</v>
       </c>
       <c r="E388">
         <v>479257</v>
@@ -8172,10 +8175,10 @@
         <v>391</v>
       </c>
       <c r="C389" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D389">
-        <v>27492023</v>
+        <v>27492273</v>
       </c>
       <c r="E389">
         <v>482142</v>
@@ -8189,10 +8192,10 @@
         <v>392</v>
       </c>
       <c r="C390" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D390">
-        <v>27575344</v>
+        <v>27575595</v>
       </c>
       <c r="E390">
         <v>484301</v>
@@ -8206,10 +8209,10 @@
         <v>393</v>
       </c>
       <c r="C391" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D391">
-        <v>27640282</v>
+        <v>27640541</v>
       </c>
       <c r="E391">
         <v>485384</v>
@@ -8223,10 +8226,10 @@
         <v>394</v>
       </c>
       <c r="C392" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D392">
-        <v>27694226</v>
+        <v>27694511</v>
       </c>
       <c r="E392">
         <v>486325</v>
@@ -8240,10 +8243,10 @@
         <v>395</v>
       </c>
       <c r="C393" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D393">
-        <v>27756624</v>
+        <v>27756970</v>
       </c>
       <c r="E393">
         <v>488081</v>
@@ -8257,13 +8260,30 @@
         <v>396</v>
       </c>
       <c r="C394" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D394">
-        <v>27826812</v>
+        <v>27826785</v>
       </c>
       <c r="E394">
         <v>490540</v>
+      </c>
+    </row>
+    <row r="395" spans="1:5">
+      <c r="A395" s="1">
+        <v>393</v>
+      </c>
+      <c r="B395" t="s">
+        <v>397</v>
+      </c>
+      <c r="C395" t="s">
+        <v>398</v>
+      </c>
+      <c r="D395">
+        <v>27896040</v>
+      </c>
+      <c r="E395">
+        <v>493098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>